<commit_message>
modified:   Input/Exam Timetable.xlsx 	modified:   __pycache__/class_def.cpython-311.pyc 	modified:   class_def.py 	modified:   main.ipynb 	modified:   main.py 	deleted:    "\347\233\243\350\200\203\346\231\202\351\226\223\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/Input/Exam Timetable.xlsx
+++ b/Input/Exam Timetable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C29518-3793-4453-B771-8E71F50E0AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7990D6F-305A-434F-BF23-3931E2D5306D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2695,8 +2695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="K114" sqref="K114:K117"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -5140,7 +5140,7 @@
     <row r="109" spans="1:11" ht="15.75" thickBot="1">
       <c r="A109" s="10"/>
       <c r="B109" s="11" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C109" s="11" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
modified:   Input/Exam Timetable.xlsx 	new file:   Input/Other Info.xlsx 	modified:   Input/Specific Examer.xlsx 	modified:   main.ipynb
</commit_message>
<xml_diff>
--- a/Input/Exam Timetable.xlsx
+++ b/Input/Exam Timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90501D85-BCBC-4300-BD57-80347071E061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6074736C-F518-4FC7-BFF3-02DF9D40F062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15034" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1898,6 +1898,12 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1907,9 +1913,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1937,25 +1940,22 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2244,16 +2244,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="N115" sqref="N115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="2" max="11" width="16.6640625" customWidth="1"/>
+    <col min="2" max="11" width="16.640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" thickBot="1">
+    <row r="1" spans="1:11" ht="14.6" thickBot="1">
       <c r="A1" s="54" t="s">
         <v>166</v>
       </c>
@@ -2268,7 +2268,7 @@
       <c r="J1" s="54"/>
       <c r="K1" s="54"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25" thickBot="1">
+    <row r="2" spans="1:11" ht="14.6" thickBot="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2301,7 +2301,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.15" thickBot="1">
+    <row r="3" spans="1:11" ht="28.75" thickBot="1">
       <c r="A3" s="48" t="s">
         <v>10</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" thickBot="1">
+    <row r="4" spans="1:11" ht="14.6" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.25" thickBot="1">
+    <row r="5" spans="1:11" ht="14.6" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.25" thickBot="1">
+    <row r="6" spans="1:11" ht="14.6" thickBot="1">
       <c r="A6" s="24" t="s">
         <v>13</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="42" thickBot="1">
+    <row r="7" spans="1:11" ht="42.9" thickBot="1">
       <c r="A7" s="48" t="s">
         <v>10</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.25" thickBot="1">
+    <row r="8" spans="1:11" ht="14.6" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" thickBot="1">
+    <row r="9" spans="1:11" ht="14.6" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="55.9" thickBot="1">
+    <row r="10" spans="1:11" ht="57" thickBot="1">
       <c r="A10" s="24" t="s">
         <v>13</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.15" thickBot="1">
+    <row r="11" spans="1:11" ht="28.75" thickBot="1">
       <c r="A11" s="48" t="s">
         <v>10</v>
       </c>
@@ -2549,16 +2549,16 @@
       <c r="E11" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-    </row>
-    <row r="12" spans="1:11" ht="14.25" thickBot="1">
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+    </row>
+    <row r="12" spans="1:11" ht="14.6" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -2566,16 +2566,16 @@
       <c r="C12" s="58"/>
       <c r="D12" s="58"/>
       <c r="E12" s="58"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
       <c r="I12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-    </row>
-    <row r="13" spans="1:11" ht="55.9" thickBot="1">
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+    </row>
+    <row r="13" spans="1:11" ht="57" thickBot="1">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -2583,16 +2583,16 @@
       <c r="C13" s="58"/>
       <c r="D13" s="58"/>
       <c r="E13" s="58"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
       <c r="I13" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-    </row>
-    <row r="14" spans="1:11" ht="55.9" thickBot="1">
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+    </row>
+    <row r="14" spans="1:11" ht="57" thickBot="1">
       <c r="A14" s="24" t="s">
         <v>13</v>
       </c>
@@ -2600,21 +2600,21 @@
       <c r="C14" s="58"/>
       <c r="D14" s="58"/>
       <c r="E14" s="58"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
       <c r="I14" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-    </row>
-    <row r="16" spans="1:11" ht="14.25" thickBot="1">
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+    </row>
+    <row r="16" spans="1:11" ht="14.6" thickBot="1">
       <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.4" thickBot="1">
+    <row r="17" spans="1:11" ht="15.45" thickBot="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="str">
         <f t="shared" ref="B17:K17" si="0">B2</f>
@@ -2657,7 +2657,7 @@
         <v>23/06/2023 (五)</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30.4" thickBot="1">
+    <row r="18" spans="1:11" ht="30.45" thickBot="1">
       <c r="A18" s="49" t="s">
         <v>31</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1">
+    <row r="19" spans="1:11" ht="15.9" thickBot="1">
       <c r="A19" s="12" t="s">
         <v>32</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="31.15" thickBot="1">
+    <row r="20" spans="1:11" ht="15.9" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>33</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="31.15" thickBot="1">
+    <row r="21" spans="1:11" ht="15.9" thickBot="1">
       <c r="A21" s="50" t="s">
         <v>35</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="30.4" thickBot="1">
+    <row r="22" spans="1:11" ht="30.45" thickBot="1">
       <c r="A22" s="49" t="s">
         <v>31</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
+    <row r="23" spans="1:11" ht="15.9" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>32</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="31.15" thickBot="1">
+    <row r="24" spans="1:11" ht="15.9" thickBot="1">
       <c r="A24" s="12" t="s">
         <v>33</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="61.9" thickBot="1">
+    <row r="25" spans="1:11" ht="46.75" thickBot="1">
       <c r="A25" s="50" t="s">
         <v>35</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30.4" thickBot="1">
+    <row r="26" spans="1:11" ht="30.45" thickBot="1">
       <c r="A26" s="49" t="s">
         <v>31</v>
       </c>
@@ -2905,10 +2905,10 @@
       <c r="E26" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
       <c r="J26" s="30" t="s">
         <v>42</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1">
+    <row r="27" spans="1:11" ht="15.9" thickBot="1">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -2924,10 +2924,10 @@
       <c r="C27" s="59"/>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
       <c r="J27" s="12" t="s">
         <v>176</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="61.9" thickBot="1">
+    <row r="28" spans="1:11" ht="46.75" thickBot="1">
       <c r="A28" s="13" t="s">
         <v>33</v>
       </c>
@@ -2943,10 +2943,10 @@
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
       <c r="J28" s="12" t="s">
         <v>175</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="61.9" thickBot="1">
+    <row r="29" spans="1:11" ht="62.15" thickBot="1">
       <c r="A29" s="50" t="s">
         <v>35</v>
       </c>
@@ -2962,10 +2962,10 @@
       <c r="C29" s="59"/>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
       <c r="J29" s="50" t="s">
         <v>90</v>
       </c>
@@ -2973,12 +2973,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1">
+    <row r="31" spans="1:11" ht="15.9" thickBot="1">
       <c r="A31" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.4" thickBot="1">
+    <row r="32" spans="1:11" ht="15.45" thickBot="1">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="str">
         <f t="shared" ref="B32:K32" si="1">B2</f>
@@ -3021,7 +3021,7 @@
         <v>23/06/2023 (五)</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="31.15" thickBot="1">
+    <row r="33" spans="1:11" ht="32.15" thickBot="1">
       <c r="A33" s="49" t="s">
         <v>31</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1">
+    <row r="34" spans="1:11" ht="15.9" thickBot="1">
       <c r="A34" s="12" t="s">
         <v>32</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="26.65" thickBot="1">
+    <row r="35" spans="1:11" ht="15.9" thickBot="1">
       <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="31.15" thickBot="1">
+    <row r="36" spans="1:11" ht="15.9" thickBot="1">
       <c r="A36" s="50" t="s">
         <v>35</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="40.9" thickBot="1">
+    <row r="37" spans="1:11" ht="40.299999999999997" thickBot="1">
       <c r="A37" s="49" t="s">
         <v>31</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1">
+    <row r="38" spans="1:11" ht="15.9" thickBot="1">
       <c r="A38" s="12" t="s">
         <v>32</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="26.65" thickBot="1">
+    <row r="39" spans="1:11" ht="15.9" thickBot="1">
       <c r="A39" s="12" t="s">
         <v>33</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="31.15" thickBot="1">
+    <row r="40" spans="1:11" ht="31.3" thickBot="1">
       <c r="A40" s="50" t="s">
         <v>35</v>
       </c>
@@ -3301,12 +3301,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30.4" thickBot="1">
+    <row r="41" spans="1:11" ht="30.45" thickBot="1">
       <c r="A41" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
       <c r="D41" s="38" t="s">
         <v>67</v>
       </c>
@@ -3316,20 +3316,20 @@
       <c r="F41" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G41" s="70"/>
+      <c r="G41" s="71"/>
       <c r="H41" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="I41" s="70"/>
-      <c r="J41" s="70"/>
-      <c r="K41" s="70"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1">
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.9" thickBot="1">
       <c r="A42" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="73"/>
-      <c r="C42" s="73"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
       <c r="D42" s="12">
         <v>30</v>
       </c>
@@ -3339,20 +3339,20 @@
       <c r="F42" s="12">
         <v>65</v>
       </c>
-      <c r="G42" s="71"/>
+      <c r="G42" s="72"/>
       <c r="H42" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="I42" s="71"/>
-      <c r="J42" s="71"/>
-      <c r="K42" s="71"/>
-    </row>
-    <row r="43" spans="1:11" ht="77.25" thickBot="1">
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+    </row>
+    <row r="43" spans="1:11" ht="62.15" thickBot="1">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="73"/>
-      <c r="C43" s="73"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="12" t="s">
         <v>164</v>
       </c>
@@ -3362,20 +3362,20 @@
       <c r="F43" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="71"/>
+      <c r="G43" s="72"/>
       <c r="H43" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="I43" s="71"/>
-      <c r="J43" s="71"/>
-      <c r="K43" s="71"/>
-    </row>
-    <row r="44" spans="1:11" ht="61.9" thickBot="1">
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="72"/>
+    </row>
+    <row r="44" spans="1:11" ht="62.15" thickBot="1">
       <c r="A44" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="73"/>
-      <c r="C44" s="73"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
       <c r="D44" s="50" t="s">
         <v>54</v>
       </c>
@@ -3385,20 +3385,20 @@
       <c r="F44" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="72"/>
+      <c r="G44" s="73"/>
       <c r="H44" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="I44" s="72"/>
-      <c r="J44" s="72"/>
-      <c r="K44" s="72"/>
-    </row>
-    <row r="46" spans="1:11" ht="15.4" thickBot="1">
+      <c r="I44" s="73"/>
+      <c r="J44" s="73"/>
+      <c r="K44" s="73"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.45" thickBot="1">
       <c r="A46" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.4" thickBot="1">
+    <row r="47" spans="1:11" ht="15.45" thickBot="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11" t="str">
         <f t="shared" ref="B47:K47" si="2">B2</f>
@@ -3441,7 +3441,7 @@
         <v>23/06/2023 (五)</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="30.4" thickBot="1">
+    <row r="48" spans="1:11" ht="30.45" thickBot="1">
       <c r="A48" s="49" t="s">
         <v>74</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.75" thickBot="1">
+    <row r="49" spans="1:11" ht="15.9" thickBot="1">
       <c r="A49" s="12" t="s">
         <v>32</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="31.15" thickBot="1">
+    <row r="50" spans="1:11" ht="28.75" thickBot="1">
       <c r="A50" s="12" t="s">
         <v>33</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="31.15" thickBot="1">
+    <row r="51" spans="1:11" ht="15.9" thickBot="1">
       <c r="A51" s="50" t="s">
         <v>35</v>
       </c>
@@ -3581,14 +3581,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30.4" thickBot="1">
+    <row r="52" spans="1:11" ht="30.45" thickBot="1">
       <c r="A52" s="49" t="s">
         <v>74</v>
       </c>
       <c r="B52" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="C52" s="76"/>
+      <c r="C52" s="77"/>
       <c r="D52" s="30" t="s">
         <v>102</v>
       </c>
@@ -3601,23 +3601,23 @@
       <c r="G52" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H52" s="60"/>
+      <c r="H52" s="62"/>
       <c r="I52" s="43" t="s">
         <v>95</v>
       </c>
       <c r="J52" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="K52" s="60"/>
-    </row>
-    <row r="53" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K52" s="62"/>
+    </row>
+    <row r="53" spans="1:11" ht="15.9" thickBot="1">
       <c r="A53" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B53" s="12">
         <v>90</v>
       </c>
-      <c r="C53" s="76"/>
+      <c r="C53" s="77"/>
       <c r="D53" s="13">
         <v>75</v>
       </c>
@@ -3630,23 +3630,23 @@
       <c r="G53" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="H53" s="61"/>
+      <c r="H53" s="63"/>
       <c r="I53" s="18">
         <v>90</v>
       </c>
       <c r="J53" s="18">
         <v>120</v>
       </c>
-      <c r="K53" s="61"/>
-    </row>
-    <row r="54" spans="1:11" ht="77.25" thickBot="1">
+      <c r="K53" s="63"/>
+    </row>
+    <row r="54" spans="1:11" ht="62.15" thickBot="1">
       <c r="A54" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B54" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C54" s="76"/>
+      <c r="C54" s="77"/>
       <c r="D54" s="15" t="s">
         <v>75</v>
       </c>
@@ -3659,23 +3659,23 @@
       <c r="G54" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="H54" s="61"/>
+      <c r="H54" s="63"/>
       <c r="I54" s="18" t="s">
         <v>132</v>
       </c>
       <c r="J54" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="K54" s="61"/>
-    </row>
-    <row r="55" spans="1:11" ht="61.9" thickBot="1">
+      <c r="K54" s="63"/>
+    </row>
+    <row r="55" spans="1:11" ht="62.15" thickBot="1">
       <c r="A55" s="50" t="s">
         <v>35</v>
       </c>
       <c r="B55" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="76"/>
+      <c r="C55" s="77"/>
       <c r="D55" s="50" t="s">
         <v>100</v>
       </c>
@@ -3688,437 +3688,437 @@
       <c r="G55" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="H55" s="62"/>
+      <c r="H55" s="64"/>
       <c r="I55" s="50" t="s">
         <v>21</v>
       </c>
       <c r="J55" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="K55" s="62"/>
-    </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K55" s="64"/>
+    </row>
+    <row r="56" spans="1:11" ht="15.9" thickBot="1">
       <c r="A56" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="60"/>
-      <c r="C56" s="60"/>
-      <c r="D56" s="60"/>
-      <c r="E56" s="60"/>
-      <c r="F56" s="60"/>
-      <c r="G56" s="60"/>
-      <c r="H56" s="60"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="62"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="62"/>
+      <c r="G56" s="62"/>
+      <c r="H56" s="62"/>
       <c r="I56" s="44" t="s">
         <v>23</v>
       </c>
       <c r="J56" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="K56" s="60"/>
-    </row>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K56" s="62"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.9" thickBot="1">
       <c r="A57" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B57" s="61"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="61"/>
-      <c r="G57" s="61"/>
-      <c r="H57" s="61"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="63"/>
+      <c r="F57" s="63"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="63"/>
       <c r="I57" s="18">
         <v>135</v>
       </c>
       <c r="J57" s="18">
         <v>150</v>
       </c>
-      <c r="K57" s="61"/>
-    </row>
-    <row r="58" spans="1:11" ht="31.15" thickBot="1">
+      <c r="K57" s="63"/>
+    </row>
+    <row r="58" spans="1:11" ht="31.3" thickBot="1">
       <c r="A58" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B58" s="61"/>
-      <c r="C58" s="61"/>
-      <c r="D58" s="61"/>
-      <c r="E58" s="61"/>
-      <c r="F58" s="61"/>
-      <c r="G58" s="61"/>
-      <c r="H58" s="61"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="63"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
       <c r="I58" s="18" t="s">
         <v>134</v>
       </c>
       <c r="J58" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="K58" s="61"/>
-    </row>
-    <row r="59" spans="1:11" ht="31.15" thickBot="1">
+      <c r="K58" s="63"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.9" thickBot="1">
       <c r="A59" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="62"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="62"/>
-      <c r="E59" s="62"/>
-      <c r="F59" s="62"/>
-      <c r="G59" s="62"/>
-      <c r="H59" s="62"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="64"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="64"/>
+      <c r="H59" s="64"/>
       <c r="I59" s="50" t="s">
         <v>79</v>
       </c>
       <c r="J59" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="K59" s="62"/>
-    </row>
-    <row r="60" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K59" s="64"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.9" thickBot="1">
       <c r="A60" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="60"/>
-      <c r="C60" s="60"/>
-      <c r="D60" s="60"/>
-      <c r="E60" s="60"/>
-      <c r="F60" s="60"/>
-      <c r="G60" s="60"/>
-      <c r="H60" s="60"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="62"/>
+      <c r="F60" s="62"/>
+      <c r="G60" s="62"/>
+      <c r="H60" s="62"/>
       <c r="I60" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="J60" s="60"/>
-      <c r="K60" s="60"/>
-    </row>
-    <row r="61" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J60" s="62"/>
+      <c r="K60" s="62"/>
+    </row>
+    <row r="61" spans="1:11" ht="15.9" thickBot="1">
       <c r="A61" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="61"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="61"/>
+      <c r="B61" s="63"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="63"/>
       <c r="I61" s="18">
         <v>60</v>
       </c>
-      <c r="J61" s="61"/>
-      <c r="K61" s="61"/>
-    </row>
-    <row r="62" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J61" s="63"/>
+      <c r="K61" s="63"/>
+    </row>
+    <row r="62" spans="1:11" ht="15.9" thickBot="1">
       <c r="A62" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B62" s="61"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="61"/>
-      <c r="G62" s="61"/>
-      <c r="H62" s="61"/>
+      <c r="B62" s="63"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="63"/>
       <c r="I62" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="J62" s="61"/>
-      <c r="K62" s="61"/>
-    </row>
-    <row r="63" spans="1:11" ht="29.65" thickBot="1">
+      <c r="J62" s="63"/>
+      <c r="K62" s="63"/>
+    </row>
+    <row r="63" spans="1:11" ht="15.9" thickBot="1">
       <c r="A63" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="62"/>
-      <c r="C63" s="62"/>
-      <c r="D63" s="62"/>
-      <c r="E63" s="62"/>
-      <c r="F63" s="62"/>
-      <c r="G63" s="62"/>
-      <c r="H63" s="62"/>
+      <c r="B63" s="64"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="64"/>
       <c r="I63" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="J63" s="62"/>
-      <c r="K63" s="62"/>
-    </row>
-    <row r="64" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J63" s="64"/>
+      <c r="K63" s="64"/>
+    </row>
+    <row r="64" spans="1:11" ht="15.9" thickBot="1">
       <c r="A64" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B64" s="60"/>
-      <c r="C64" s="60"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="60"/>
-      <c r="F64" s="60"/>
-      <c r="G64" s="60"/>
-      <c r="H64" s="60"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="62"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="62"/>
       <c r="I64" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="J64" s="60"/>
-      <c r="K64" s="60"/>
-    </row>
-    <row r="65" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J64" s="62"/>
+      <c r="K64" s="62"/>
+    </row>
+    <row r="65" spans="1:11" ht="15.9" thickBot="1">
       <c r="A65" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B65" s="61"/>
-      <c r="C65" s="61"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="61"/>
-      <c r="G65" s="61"/>
-      <c r="H65" s="61"/>
+      <c r="B65" s="63"/>
+      <c r="C65" s="63"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="63"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="63"/>
+      <c r="H65" s="63"/>
       <c r="I65" s="18">
         <v>120</v>
       </c>
-      <c r="J65" s="61"/>
-      <c r="K65" s="61"/>
-    </row>
-    <row r="66" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J65" s="63"/>
+      <c r="K65" s="63"/>
+    </row>
+    <row r="66" spans="1:11" ht="15.9" thickBot="1">
       <c r="A66" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B66" s="61"/>
-      <c r="C66" s="61"/>
-      <c r="D66" s="61"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="61"/>
-      <c r="G66" s="61"/>
-      <c r="H66" s="61"/>
+      <c r="B66" s="63"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="63"/>
+      <c r="F66" s="63"/>
+      <c r="G66" s="63"/>
+      <c r="H66" s="63"/>
       <c r="I66" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="J66" s="61"/>
-      <c r="K66" s="61"/>
-    </row>
-    <row r="67" spans="1:11" ht="31.15" thickBot="1">
+      <c r="J66" s="63"/>
+      <c r="K66" s="63"/>
+    </row>
+    <row r="67" spans="1:11" ht="15.9" thickBot="1">
       <c r="A67" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B67" s="62"/>
-      <c r="C67" s="62"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="62"/>
-      <c r="F67" s="62"/>
-      <c r="G67" s="62"/>
-      <c r="H67" s="62"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="64"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="64"/>
       <c r="I67" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="J67" s="62"/>
-      <c r="K67" s="62"/>
-    </row>
-    <row r="68" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J67" s="64"/>
+      <c r="K67" s="64"/>
+    </row>
+    <row r="68" spans="1:11" ht="15.9" thickBot="1">
       <c r="A68" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="60"/>
-      <c r="C68" s="60"/>
-      <c r="D68" s="60"/>
-      <c r="E68" s="60"/>
-      <c r="F68" s="60"/>
-      <c r="G68" s="60"/>
-      <c r="H68" s="60"/>
+      <c r="B68" s="62"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="62"/>
+      <c r="F68" s="62"/>
+      <c r="G68" s="62"/>
+      <c r="H68" s="62"/>
       <c r="I68" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="J68" s="60"/>
-      <c r="K68" s="60"/>
-    </row>
-    <row r="69" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J68" s="62"/>
+      <c r="K68" s="62"/>
+    </row>
+    <row r="69" spans="1:11" ht="15.9" thickBot="1">
       <c r="A69" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B69" s="61"/>
-      <c r="C69" s="61"/>
-      <c r="D69" s="61"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="61"/>
-      <c r="G69" s="61"/>
-      <c r="H69" s="61"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="63"/>
+      <c r="D69" s="63"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="63"/>
+      <c r="H69" s="63"/>
       <c r="I69" s="18">
         <v>90</v>
       </c>
-      <c r="J69" s="61"/>
-      <c r="K69" s="61"/>
-    </row>
-    <row r="70" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J69" s="63"/>
+      <c r="K69" s="63"/>
+    </row>
+    <row r="70" spans="1:11" ht="15.9" thickBot="1">
       <c r="A70" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B70" s="61"/>
-      <c r="C70" s="61"/>
-      <c r="D70" s="61"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="61"/>
-      <c r="G70" s="61"/>
-      <c r="H70" s="61"/>
+      <c r="B70" s="63"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="63"/>
+      <c r="E70" s="63"/>
+      <c r="F70" s="63"/>
+      <c r="G70" s="63"/>
+      <c r="H70" s="63"/>
       <c r="I70" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="J70" s="61"/>
-      <c r="K70" s="61"/>
-    </row>
-    <row r="71" spans="1:11" ht="31.15" thickBot="1">
+      <c r="J70" s="63"/>
+      <c r="K70" s="63"/>
+    </row>
+    <row r="71" spans="1:11" ht="15.9" thickBot="1">
       <c r="A71" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="62"/>
-      <c r="C71" s="62"/>
-      <c r="D71" s="62"/>
-      <c r="E71" s="62"/>
-      <c r="F71" s="62"/>
-      <c r="G71" s="62"/>
-      <c r="H71" s="62"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="64"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="64"/>
+      <c r="H71" s="64"/>
       <c r="I71" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="J71" s="62"/>
-      <c r="K71" s="62"/>
-    </row>
-    <row r="72" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J71" s="64"/>
+      <c r="K71" s="64"/>
+    </row>
+    <row r="72" spans="1:11" ht="15.9" thickBot="1">
       <c r="A72" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="60"/>
-      <c r="C72" s="60"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="60"/>
-      <c r="G72" s="60"/>
-      <c r="H72" s="60"/>
+      <c r="B72" s="62"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="62"/>
+      <c r="E72" s="62"/>
+      <c r="F72" s="62"/>
+      <c r="G72" s="62"/>
+      <c r="H72" s="62"/>
       <c r="I72" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="J72" s="60"/>
-      <c r="K72" s="60"/>
-    </row>
-    <row r="73" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J72" s="62"/>
+      <c r="K72" s="62"/>
+    </row>
+    <row r="73" spans="1:11" ht="15.9" thickBot="1">
       <c r="A73" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B73" s="61"/>
-      <c r="C73" s="61"/>
-      <c r="D73" s="61"/>
-      <c r="E73" s="61"/>
-      <c r="F73" s="61"/>
-      <c r="G73" s="61"/>
-      <c r="H73" s="61"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="63"/>
+      <c r="F73" s="63"/>
+      <c r="G73" s="63"/>
+      <c r="H73" s="63"/>
       <c r="I73" s="18">
         <v>75</v>
       </c>
-      <c r="J73" s="61"/>
-      <c r="K73" s="61"/>
-    </row>
-    <row r="74" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J73" s="63"/>
+      <c r="K73" s="63"/>
+    </row>
+    <row r="74" spans="1:11" ht="15.9" thickBot="1">
       <c r="A74" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B74" s="61"/>
-      <c r="C74" s="61"/>
-      <c r="D74" s="61"/>
-      <c r="E74" s="61"/>
-      <c r="F74" s="61"/>
-      <c r="G74" s="61"/>
-      <c r="H74" s="61"/>
+      <c r="B74" s="63"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="63"/>
+      <c r="E74" s="63"/>
+      <c r="F74" s="63"/>
+      <c r="G74" s="63"/>
+      <c r="H74" s="63"/>
       <c r="I74" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J74" s="61"/>
-      <c r="K74" s="61"/>
-    </row>
-    <row r="75" spans="1:11" ht="31.15" thickBot="1">
+      <c r="J74" s="63"/>
+      <c r="K74" s="63"/>
+    </row>
+    <row r="75" spans="1:11" ht="31.3" thickBot="1">
       <c r="A75" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B75" s="62"/>
-      <c r="C75" s="62"/>
-      <c r="D75" s="62"/>
-      <c r="E75" s="62"/>
-      <c r="F75" s="62"/>
-      <c r="G75" s="62"/>
-      <c r="H75" s="62"/>
+      <c r="B75" s="64"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="64"/>
+      <c r="H75" s="64"/>
       <c r="I75" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="J75" s="62"/>
-      <c r="K75" s="62"/>
-    </row>
-    <row r="76" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J75" s="64"/>
+      <c r="K75" s="64"/>
+    </row>
+    <row r="76" spans="1:11" ht="15.9" thickBot="1">
       <c r="A76" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="60"/>
-      <c r="C76" s="74"/>
-      <c r="D76" s="77"/>
-      <c r="E76" s="60"/>
-      <c r="F76" s="60"/>
-      <c r="G76" s="60"/>
-      <c r="H76" s="75"/>
+      <c r="B76" s="62"/>
+      <c r="C76" s="78"/>
+      <c r="D76" s="74"/>
+      <c r="E76" s="62"/>
+      <c r="F76" s="62"/>
+      <c r="G76" s="62"/>
+      <c r="H76" s="79"/>
       <c r="I76" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="J76" s="76"/>
-      <c r="K76" s="76"/>
-    </row>
-    <row r="77" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J76" s="77"/>
+      <c r="K76" s="77"/>
+    </row>
+    <row r="77" spans="1:11" ht="15.9" thickBot="1">
       <c r="A77" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="61"/>
-      <c r="C77" s="74"/>
-      <c r="D77" s="78"/>
-      <c r="E77" s="61"/>
-      <c r="F77" s="61"/>
-      <c r="G77" s="61"/>
-      <c r="H77" s="75"/>
+      <c r="B77" s="63"/>
+      <c r="C77" s="78"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="63"/>
+      <c r="F77" s="63"/>
+      <c r="G77" s="63"/>
+      <c r="H77" s="79"/>
       <c r="I77" s="18">
         <v>90</v>
       </c>
-      <c r="J77" s="76"/>
-      <c r="K77" s="76"/>
-    </row>
-    <row r="78" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J77" s="77"/>
+      <c r="K77" s="77"/>
+    </row>
+    <row r="78" spans="1:11" ht="15.9" thickBot="1">
       <c r="A78" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="61"/>
-      <c r="C78" s="74"/>
-      <c r="D78" s="78"/>
-      <c r="E78" s="61"/>
-      <c r="F78" s="61"/>
-      <c r="G78" s="61"/>
-      <c r="H78" s="75"/>
+      <c r="B78" s="63"/>
+      <c r="C78" s="78"/>
+      <c r="D78" s="75"/>
+      <c r="E78" s="63"/>
+      <c r="F78" s="63"/>
+      <c r="G78" s="63"/>
+      <c r="H78" s="79"/>
       <c r="I78" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="J78" s="76"/>
-      <c r="K78" s="76"/>
-    </row>
-    <row r="79" spans="1:11" ht="31.15" thickBot="1">
+      <c r="J78" s="77"/>
+      <c r="K78" s="77"/>
+    </row>
+    <row r="79" spans="1:11" ht="31.3" thickBot="1">
       <c r="A79" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="62"/>
-      <c r="C79" s="74"/>
-      <c r="D79" s="79"/>
-      <c r="E79" s="62"/>
-      <c r="F79" s="62"/>
-      <c r="G79" s="62"/>
-      <c r="H79" s="75"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="78"/>
+      <c r="D79" s="76"/>
+      <c r="E79" s="64"/>
+      <c r="F79" s="64"/>
+      <c r="G79" s="64"/>
+      <c r="H79" s="79"/>
       <c r="I79" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="J79" s="76"/>
-      <c r="K79" s="76"/>
-    </row>
-    <row r="81" spans="1:11" ht="14.25" thickBot="1">
+      <c r="J79" s="77"/>
+      <c r="K79" s="77"/>
+    </row>
+    <row r="81" spans="1:11" ht="14.6" thickBot="1">
       <c r="A81" s="19" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15.4" thickBot="1">
+    <row r="82" spans="1:11" ht="15.45" thickBot="1">
       <c r="A82" s="10"/>
       <c r="B82" s="11" t="str">
         <f t="shared" ref="B82:K82" si="3">B2</f>
@@ -4161,7 +4161,7 @@
         <v>23/06/2023 (五)</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="30.4" thickBot="1">
+    <row r="83" spans="1:11" ht="30.45" thickBot="1">
       <c r="A83" s="49" t="s">
         <v>74</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15.4">
+    <row r="84" spans="1:11" ht="15.45">
       <c r="A84" s="12" t="s">
         <v>32</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="31.15" thickBot="1">
+    <row r="85" spans="1:11" ht="31.3" thickBot="1">
       <c r="A85" s="12" t="s">
         <v>33</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="31.15" thickBot="1">
+    <row r="86" spans="1:11" ht="15.9" thickBot="1">
       <c r="A86" s="50" t="s">
         <v>35</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="30.4" thickBot="1">
+    <row r="87" spans="1:11" ht="30.45" thickBot="1">
       <c r="A87" s="49" t="s">
         <v>74</v>
       </c>
@@ -4332,9 +4332,9 @@
       <c r="J87" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="K87" s="60"/>
-    </row>
-    <row r="88" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K87" s="62"/>
+    </row>
+    <row r="88" spans="1:11" ht="15.9" thickBot="1">
       <c r="A88" s="12" t="s">
         <v>32</v>
       </c>
@@ -4365,9 +4365,9 @@
       <c r="J88" s="12">
         <v>120</v>
       </c>
-      <c r="K88" s="61"/>
-    </row>
-    <row r="89" spans="1:11" ht="77.25" thickBot="1">
+      <c r="K88" s="63"/>
+    </row>
+    <row r="89" spans="1:11" ht="62.15" thickBot="1">
       <c r="A89" s="12" t="s">
         <v>33</v>
       </c>
@@ -4398,9 +4398,9 @@
       <c r="J89" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="K89" s="61"/>
-    </row>
-    <row r="90" spans="1:11" ht="61.9" thickBot="1">
+      <c r="K89" s="63"/>
+    </row>
+    <row r="90" spans="1:11" ht="62.15" thickBot="1">
       <c r="A90" s="50" t="s">
         <v>35</v>
       </c>
@@ -4431,17 +4431,17 @@
       <c r="J90" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="K90" s="62"/>
-    </row>
-    <row r="91" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K90" s="64"/>
+    </row>
+    <row r="91" spans="1:11" ht="15.9" thickBot="1">
       <c r="A91" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B91" s="60"/>
-      <c r="C91" s="60"/>
-      <c r="D91" s="60"/>
-      <c r="E91" s="60"/>
-      <c r="F91" s="60"/>
+      <c r="B91" s="62"/>
+      <c r="C91" s="62"/>
+      <c r="D91" s="62"/>
+      <c r="E91" s="62"/>
+      <c r="F91" s="62"/>
       <c r="G91" s="51" t="s">
         <v>96</v>
       </c>
@@ -4451,18 +4451,18 @@
       <c r="I91" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="J91" s="60"/>
-      <c r="K91" s="60"/>
-    </row>
-    <row r="92" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J91" s="62"/>
+      <c r="K91" s="62"/>
+    </row>
+    <row r="92" spans="1:11" ht="15.9" thickBot="1">
       <c r="A92" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B92" s="61"/>
-      <c r="C92" s="61"/>
-      <c r="D92" s="61"/>
-      <c r="E92" s="61"/>
-      <c r="F92" s="61"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="63"/>
+      <c r="E92" s="63"/>
+      <c r="F92" s="63"/>
       <c r="G92" s="12">
         <v>75</v>
       </c>
@@ -4472,18 +4472,18 @@
       <c r="I92" s="12">
         <v>120</v>
       </c>
-      <c r="J92" s="61"/>
-      <c r="K92" s="61"/>
-    </row>
-    <row r="93" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J92" s="63"/>
+      <c r="K92" s="63"/>
+    </row>
+    <row r="93" spans="1:11" ht="15.9" thickBot="1">
       <c r="A93" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B93" s="61"/>
-      <c r="C93" s="61"/>
-      <c r="D93" s="61"/>
-      <c r="E93" s="61"/>
-      <c r="F93" s="61"/>
+      <c r="B93" s="63"/>
+      <c r="C93" s="63"/>
+      <c r="D93" s="63"/>
+      <c r="E93" s="63"/>
+      <c r="F93" s="63"/>
       <c r="G93" s="13" t="s">
         <v>144</v>
       </c>
@@ -4493,18 +4493,18 @@
       <c r="I93" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="J93" s="61"/>
-      <c r="K93" s="61"/>
-    </row>
-    <row r="94" spans="1:11" ht="31.15" thickBot="1">
+      <c r="J93" s="63"/>
+      <c r="K93" s="63"/>
+    </row>
+    <row r="94" spans="1:11" ht="15.9" thickBot="1">
       <c r="A94" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B94" s="62"/>
-      <c r="C94" s="62"/>
-      <c r="D94" s="62"/>
-      <c r="E94" s="62"/>
-      <c r="F94" s="62"/>
+      <c r="B94" s="64"/>
+      <c r="C94" s="64"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="64"/>
+      <c r="F94" s="64"/>
       <c r="G94" s="50" t="s">
         <v>20</v>
       </c>
@@ -4514,220 +4514,222 @@
       <c r="I94" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="J94" s="62"/>
-      <c r="K94" s="62"/>
-    </row>
-    <row r="95" spans="1:11" ht="15.75" thickBot="1">
+      <c r="J94" s="64"/>
+      <c r="K94" s="64"/>
+    </row>
+    <row r="95" spans="1:11" ht="15.9" thickBot="1">
       <c r="A95" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B95" s="60"/>
+      <c r="B95" s="62"/>
       <c r="C95" s="45"/>
-      <c r="D95" s="60"/>
-      <c r="E95" s="60"/>
-      <c r="F95" s="60"/>
+      <c r="D95" s="62"/>
+      <c r="E95" s="62"/>
+      <c r="F95" s="62"/>
       <c r="G95" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="H95" s="76"/>
-      <c r="I95" s="60"/>
-      <c r="J95" s="60"/>
-      <c r="K95" s="60"/>
-    </row>
-    <row r="96" spans="1:11" ht="15.75" thickBot="1">
+      <c r="H95" s="77"/>
+      <c r="I95" s="62"/>
+      <c r="J95" s="62"/>
+      <c r="K95" s="62"/>
+    </row>
+    <row r="96" spans="1:11" ht="15.9" thickBot="1">
       <c r="A96" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B96" s="61"/>
+      <c r="B96" s="63"/>
       <c r="C96" s="46"/>
-      <c r="D96" s="61"/>
-      <c r="E96" s="61"/>
-      <c r="F96" s="61"/>
+      <c r="D96" s="63"/>
+      <c r="E96" s="63"/>
+      <c r="F96" s="63"/>
       <c r="G96" s="12">
         <v>150</v>
       </c>
-      <c r="H96" s="76"/>
-      <c r="I96" s="61"/>
-      <c r="J96" s="61"/>
-      <c r="K96" s="61"/>
-    </row>
-    <row r="97" spans="1:11" ht="15.75" thickBot="1">
+      <c r="H96" s="77"/>
+      <c r="I96" s="63"/>
+      <c r="J96" s="63"/>
+      <c r="K96" s="63"/>
+    </row>
+    <row r="97" spans="1:11" ht="15.9" thickBot="1">
       <c r="A97" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B97" s="61"/>
+      <c r="B97" s="63"/>
       <c r="C97" s="46"/>
-      <c r="D97" s="61"/>
-      <c r="E97" s="61"/>
-      <c r="F97" s="61"/>
+      <c r="D97" s="63"/>
+      <c r="E97" s="63"/>
+      <c r="F97" s="63"/>
       <c r="G97" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="H97" s="76"/>
-      <c r="I97" s="61"/>
-      <c r="J97" s="61"/>
-      <c r="K97" s="61"/>
-    </row>
-    <row r="98" spans="1:11" ht="31.15" thickBot="1">
+      <c r="H97" s="77"/>
+      <c r="I97" s="63"/>
+      <c r="J97" s="63"/>
+      <c r="K97" s="63"/>
+    </row>
+    <row r="98" spans="1:11" ht="15.9" thickBot="1">
       <c r="A98" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B98" s="62"/>
+      <c r="B98" s="64"/>
       <c r="C98" s="47"/>
-      <c r="D98" s="62"/>
-      <c r="E98" s="62"/>
-      <c r="F98" s="62"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
+      <c r="F98" s="64"/>
       <c r="G98" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="H98" s="76"/>
-      <c r="I98" s="62"/>
-      <c r="J98" s="62"/>
-      <c r="K98" s="62"/>
-    </row>
-    <row r="99" spans="1:11" ht="15.75" thickBot="1">
+      <c r="H98" s="77"/>
+      <c r="I98" s="64"/>
+      <c r="J98" s="64"/>
+      <c r="K98" s="64"/>
+    </row>
+    <row r="99" spans="1:11" ht="15.9" thickBot="1">
       <c r="A99" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B99" s="60"/>
-      <c r="C99" s="60"/>
-      <c r="D99" s="60"/>
-      <c r="E99" s="60"/>
-      <c r="F99" s="60"/>
+      <c r="B99" s="62"/>
+      <c r="C99" s="62"/>
+      <c r="D99" s="62"/>
+      <c r="E99" s="62"/>
+      <c r="F99" s="62"/>
       <c r="G99" s="30" t="s">
         <v>127</v>
       </c>
       <c r="H99" s="80"/>
-      <c r="I99" s="60"/>
-      <c r="J99" s="60"/>
+      <c r="I99" s="62"/>
+      <c r="J99" s="62"/>
       <c r="K99" s="80"/>
     </row>
-    <row r="100" spans="1:11" ht="15.75" thickBot="1">
+    <row r="100" spans="1:11" ht="15.9" thickBot="1">
       <c r="A100" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B100" s="61"/>
-      <c r="C100" s="61"/>
-      <c r="D100" s="61"/>
-      <c r="E100" s="61"/>
-      <c r="F100" s="61"/>
+      <c r="B100" s="63"/>
+      <c r="C100" s="63"/>
+      <c r="D100" s="63"/>
+      <c r="E100" s="63"/>
+      <c r="F100" s="63"/>
       <c r="G100" s="12">
         <v>105</v>
       </c>
       <c r="H100" s="80"/>
-      <c r="I100" s="61"/>
-      <c r="J100" s="61"/>
+      <c r="I100" s="63"/>
+      <c r="J100" s="63"/>
       <c r="K100" s="80"/>
     </row>
-    <row r="101" spans="1:11" ht="15.75" thickBot="1">
+    <row r="101" spans="1:11" ht="15.9" thickBot="1">
       <c r="A101" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B101" s="61"/>
-      <c r="C101" s="61"/>
-      <c r="D101" s="61"/>
-      <c r="E101" s="61"/>
-      <c r="F101" s="61"/>
+      <c r="B101" s="63"/>
+      <c r="C101" s="63"/>
+      <c r="D101" s="63"/>
+      <c r="E101" s="63"/>
+      <c r="F101" s="63"/>
       <c r="G101" s="12" t="s">
         <v>143</v>
       </c>
       <c r="H101" s="80"/>
-      <c r="I101" s="61"/>
-      <c r="J101" s="61"/>
+      <c r="I101" s="63"/>
+      <c r="J101" s="63"/>
       <c r="K101" s="80"/>
     </row>
-    <row r="102" spans="1:11" ht="31.15" thickBot="1">
+    <row r="102" spans="1:11" ht="31.3" thickBot="1">
       <c r="A102" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B102" s="62"/>
-      <c r="C102" s="62"/>
-      <c r="D102" s="62"/>
-      <c r="E102" s="62"/>
-      <c r="F102" s="62"/>
+      <c r="B102" s="64"/>
+      <c r="C102" s="64"/>
+      <c r="D102" s="64"/>
+      <c r="E102" s="64"/>
+      <c r="F102" s="64"/>
       <c r="G102" s="50" t="s">
         <v>119</v>
       </c>
       <c r="H102" s="80"/>
-      <c r="I102" s="62"/>
-      <c r="J102" s="62"/>
+      <c r="I102" s="64"/>
+      <c r="J102" s="64"/>
       <c r="K102" s="80"/>
     </row>
-    <row r="103" spans="1:11" ht="15.75" thickBot="1">
+    <row r="103" spans="1:11" ht="15.9" thickBot="1">
       <c r="A103" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B103" s="76"/>
-      <c r="C103" s="76"/>
-      <c r="D103" s="76"/>
-      <c r="E103" s="76"/>
-      <c r="F103" s="76"/>
+      <c r="B103" s="77"/>
+      <c r="C103" s="77"/>
+      <c r="D103" s="77"/>
+      <c r="E103" s="77"/>
+      <c r="F103" s="77"/>
       <c r="G103" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="H103" s="76"/>
-      <c r="I103" s="76"/>
-      <c r="J103" s="76"/>
-      <c r="K103" s="76"/>
-    </row>
-    <row r="104" spans="1:11" ht="15.75" thickBot="1">
+      <c r="H103" s="77"/>
+      <c r="I103" s="77"/>
+      <c r="J103" s="77"/>
+      <c r="K103" s="77"/>
+    </row>
+    <row r="104" spans="1:11" ht="15.9" thickBot="1">
       <c r="A104" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B104" s="76"/>
-      <c r="C104" s="76"/>
-      <c r="D104" s="76"/>
-      <c r="E104" s="76"/>
-      <c r="F104" s="76"/>
+      <c r="B104" s="77"/>
+      <c r="C104" s="77"/>
+      <c r="D104" s="77"/>
+      <c r="E104" s="77"/>
+      <c r="F104" s="77"/>
       <c r="G104" s="12">
         <v>135</v>
       </c>
-      <c r="H104" s="76"/>
-      <c r="I104" s="76"/>
-      <c r="J104" s="76"/>
-      <c r="K104" s="76"/>
-    </row>
-    <row r="105" spans="1:11" ht="15.75" thickBot="1">
+      <c r="H104" s="77"/>
+      <c r="I104" s="77"/>
+      <c r="J104" s="77"/>
+      <c r="K104" s="77"/>
+    </row>
+    <row r="105" spans="1:11" ht="15.9" thickBot="1">
       <c r="A105" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B105" s="76"/>
-      <c r="C105" s="76"/>
-      <c r="D105" s="76"/>
-      <c r="E105" s="76"/>
-      <c r="F105" s="76"/>
+      <c r="B105" s="77"/>
+      <c r="C105" s="77"/>
+      <c r="D105" s="77"/>
+      <c r="E105" s="77"/>
+      <c r="F105" s="77"/>
       <c r="G105" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="H105" s="76"/>
-      <c r="I105" s="76"/>
-      <c r="J105" s="76"/>
-      <c r="K105" s="76"/>
-    </row>
-    <row r="106" spans="1:11" ht="31.15" thickBot="1">
+      <c r="H105" s="77"/>
+      <c r="I105" s="77"/>
+      <c r="J105" s="77"/>
+      <c r="K105" s="77"/>
+    </row>
+    <row r="106" spans="1:11" ht="31.3" thickBot="1">
       <c r="A106" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B106" s="76"/>
-      <c r="C106" s="76"/>
-      <c r="D106" s="76"/>
-      <c r="E106" s="76"/>
-      <c r="F106" s="76"/>
+      <c r="B106" s="77"/>
+      <c r="C106" s="77"/>
+      <c r="D106" s="77"/>
+      <c r="E106" s="77"/>
+      <c r="F106" s="77"/>
       <c r="G106" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="H106" s="76"/>
-      <c r="I106" s="76"/>
-      <c r="J106" s="76"/>
-      <c r="K106" s="76"/>
+      <c r="H106" s="77"/>
+      <c r="I106" s="77"/>
+      <c r="J106" s="77"/>
+      <c r="K106" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="129">
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="K87:K90"/>
+    <mergeCell ref="K91:K94"/>
+    <mergeCell ref="J91:J94"/>
+    <mergeCell ref="H72:H75"/>
+    <mergeCell ref="K103:K106"/>
+    <mergeCell ref="I99:I102"/>
+    <mergeCell ref="J99:J102"/>
     <mergeCell ref="H103:H106"/>
     <mergeCell ref="I103:I106"/>
     <mergeCell ref="J103:J106"/>
@@ -4740,13 +4742,9 @@
     <mergeCell ref="G64:G67"/>
     <mergeCell ref="G68:G71"/>
     <mergeCell ref="H64:H67"/>
-    <mergeCell ref="K87:K90"/>
-    <mergeCell ref="K91:K94"/>
-    <mergeCell ref="J91:J94"/>
-    <mergeCell ref="H72:H75"/>
-    <mergeCell ref="K103:K106"/>
-    <mergeCell ref="I99:I102"/>
-    <mergeCell ref="J99:J102"/>
+    <mergeCell ref="H76:H79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="K76:K79"/>
     <mergeCell ref="J95:J98"/>
     <mergeCell ref="H95:H98"/>
     <mergeCell ref="I95:I98"/>
@@ -4759,8 +4757,6 @@
     <mergeCell ref="D103:D106"/>
     <mergeCell ref="E103:E106"/>
     <mergeCell ref="F103:F106"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="D76:D79"/>
     <mergeCell ref="B91:B94"/>
     <mergeCell ref="B99:B102"/>
     <mergeCell ref="C99:C102"/>
@@ -4774,7 +4770,6 @@
     <mergeCell ref="D91:D94"/>
     <mergeCell ref="E91:E94"/>
     <mergeCell ref="F91:F94"/>
-    <mergeCell ref="D72:D75"/>
     <mergeCell ref="E72:E75"/>
     <mergeCell ref="F72:F75"/>
     <mergeCell ref="G72:G75"/>
@@ -4783,9 +4778,8 @@
     <mergeCell ref="G76:G79"/>
     <mergeCell ref="C72:C75"/>
     <mergeCell ref="C76:C79"/>
-    <mergeCell ref="H76:H79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="D76:D79"/>
     <mergeCell ref="K72:K75"/>
     <mergeCell ref="C52:C55"/>
     <mergeCell ref="B56:B59"/>
@@ -4806,6 +4800,10 @@
     <mergeCell ref="B72:B75"/>
     <mergeCell ref="C64:C67"/>
     <mergeCell ref="C68:C71"/>
+    <mergeCell ref="H60:H63"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="D72:D75"/>
     <mergeCell ref="K11:K14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="G11:G14"/>
@@ -4819,9 +4817,11 @@
     <mergeCell ref="J41:J44"/>
     <mergeCell ref="K41:K44"/>
     <mergeCell ref="G41:G44"/>
-    <mergeCell ref="H60:H63"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="D26:D29"/>

</xml_diff>

<commit_message>
modified:   Input/Exam Timetable.xlsx 	modified:   class_def.py 	modified:   main.ipynb
</commit_message>
<xml_diff>
--- a/Input/Exam Timetable.xlsx
+++ b/Input/Exam Timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6074736C-F518-4FC7-BFF3-02DF9D40F062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D860A03-A8C7-431E-9A69-62BA3C38903F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15034" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,39 +94,14 @@
     <t>404, 405, 406, 407</t>
   </si>
   <si>
-    <t>8:30a.m.-9:30a.m.</t>
-  </si>
-  <si>
-    <t>8:30a.m.-9:45a.m.</t>
-  </si>
-  <si>
-    <t>8:30a.m.-10:00a.m.</t>
-  </si>
-  <si>
     <t>數學 II</t>
   </si>
   <si>
     <t>中國歷史</t>
-  </si>
-  <si>
-    <t>10:00a.m.-11:10a.m.</t>
-  </si>
-  <si>
-    <t>10:00a.m.-10:45a.m.</t>
-  </si>
-  <si>
-    <t>10:00a.m.-11:00a.m.</t>
-  </si>
-  <si>
-    <t>10:30a.m.-11:20a.m.</t>
   </si>
   <si>
     <t>English IV
 ( Speaking )</t>
-  </si>
-  <si>
-    <t>10:15a.m.-10:40a.m.
-10:50a.m.-11:20a.m.</t>
   </si>
   <si>
     <r>
@@ -350,12 +325,6 @@
     <t>606, 607, 401, 402, 403</t>
   </si>
   <si>
-    <t>8:30a.m.-9:10a.m.</t>
-  </si>
-  <si>
-    <t>8:30a.m.-9:15a.m.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -378,33 +347,6 @@
     </r>
   </si>
   <si>
-    <t>10:15a.m.-11:30a.m.</t>
-  </si>
-  <si>
-    <t>10:15a.m.-10:45a.m.</t>
-  </si>
-  <si>
-    <t>9:45a.m.-10:55a.m.</t>
-  </si>
-  <si>
-    <t>9:45a.m.-10:30a.m.</t>
-  </si>
-  <si>
-    <t>10:30a.m.-10:55a.m.</t>
-  </si>
-  <si>
-    <t>9:45a.m.-10:45a.m.</t>
-  </si>
-  <si>
-    <t>12:00p.m.-12:30p.m.</t>
-  </si>
-  <si>
-    <t>11:15a.m.-11:50a.m.</t>
-  </si>
-  <si>
-    <t>11:30a.m.-12:35p.m.</t>
-  </si>
-  <si>
     <t>TSA
 中文寫作</t>
   </si>
@@ -577,12 +519,6 @@
 ( Reading )</t>
   </si>
   <si>
-    <t>8:30a.m.-10:45a.m.</t>
-  </si>
-  <si>
-    <t>8:30a.m.-10:30a.m.</t>
-  </si>
-  <si>
     <t>Art Room(4ABCD)</t>
   </si>
   <si>
@@ -611,43 +547,6 @@
     <t>視覺藝術</t>
   </si>
   <si>
-    <t>10:15a.m.-11:05am
-11:15a.m.-12:05pm</t>
-  </si>
-  <si>
-    <t>8:30a.m.-9:40a.m.</t>
-  </si>
-  <si>
-    <t>10:00a.m.-11:15a.m.</t>
-  </si>
-  <si>
-    <t>10:15a.m.-11:15a.m.</t>
-  </si>
-  <si>
-    <t>10:30a.m.-11:25a.m.</t>
-  </si>
-  <si>
-    <t>9:45a.m.-10:35a.m.
-10:45a.m.-11:35a.m.</t>
-  </si>
-  <si>
-    <t>11:15a.m.-12:05p.m.
-11:25a.m.-12:20p.m.</t>
-  </si>
-  <si>
-    <t>10:30a.m.-11:30a.m.</t>
-  </si>
-  <si>
-    <t>11:30a.m.-12:10p.m.
-11:40a.m.-12:25p.m.</t>
-  </si>
-  <si>
-    <t>8:30a.m.-11:00a.m.</t>
-  </si>
-  <si>
-    <t>8:30a.m.-11:30a.m.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -675,18 +574,6 @@
     <t>ICT</t>
   </si>
   <si>
-    <t>10:30a.m.-11:45a.m.</t>
-  </si>
-  <si>
-    <t>11:15a.m.-12:45p.m</t>
-  </si>
-  <si>
-    <t>11:15a.m.-12:30p.m.</t>
-  </si>
-  <si>
-    <t>11:00a.m.-12:00p.m.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -733,9 +620,6 @@
     </r>
   </si>
   <si>
-    <t>10:00a.m.-12:00p.m.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -757,13 +641,6 @@
     </r>
   </si>
   <si>
-    <t>10:30a.m.-11:05a.m.
-10:40a.m.-11:25a.m.</t>
-  </si>
-  <si>
-    <t>10:00a.m.-11:30a.m.</t>
-  </si>
-  <si>
     <t>BAFS II</t>
   </si>
   <si>
@@ -827,9 +704,6 @@
     </r>
   </si>
   <si>
-    <t>8:30a.m.-12:30p.m.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -879,18 +753,6 @@
     <t>605 (5E)</t>
   </si>
   <si>
-    <t>10:30a.m.-12:15p.m.</t>
-  </si>
-  <si>
-    <t>11:00a.m.-12:30p.m.</t>
-  </si>
-  <si>
-    <t>11:15a.m.-12:45p.m.</t>
-  </si>
-  <si>
-    <t>10:15a.m.-12:45p.m.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -979,13 +841,6 @@
       </rPr>
       <t xml:space="preserve"> II</t>
     </r>
-  </si>
-  <si>
-    <t>11:00a.m.-11:45a.m.
-11:10a.m.-12:05p.m.</t>
-  </si>
-  <si>
-    <t>10:15a.m.-12:30p.m.</t>
   </si>
   <si>
     <t>501(4A)</t>
@@ -1355,13 +1210,6 @@
     <t>中一級 1A: 404, 1B: 405, 1C: 406, 1D: 407</t>
   </si>
   <si>
-    <t>12:05p.m.-1:05p.m.
-12:15p.m.-1:25p.m.</t>
-  </si>
-  <si>
-    <t>11:00a.m.-1:00p.m.</t>
-  </si>
-  <si>
     <t>HALL&lt;2&gt;, 301[p], 601[p], 302, 303, 304, 305, 602, 603, 604, 605</t>
   </si>
   <si>
@@ -1408,6 +1256,159 @@
   </si>
   <si>
     <t>45/55</t>
+  </si>
+  <si>
+    <t>8:30-9:30</t>
+  </si>
+  <si>
+    <t>8:30-9:45</t>
+  </si>
+  <si>
+    <t>8:30-10:00</t>
+  </si>
+  <si>
+    <t>10:00-11:10</t>
+  </si>
+  <si>
+    <t>10:00-10:45</t>
+  </si>
+  <si>
+    <t>10:00-11:00</t>
+  </si>
+  <si>
+    <t>10:15-10:40
+10:50-11:20</t>
+  </si>
+  <si>
+    <t>10:30-11:20</t>
+  </si>
+  <si>
+    <t>10:50-12:40
+12:00-12:55</t>
+  </si>
+  <si>
+    <t>8:30-9:40</t>
+  </si>
+  <si>
+    <t>8:30-9:15</t>
+  </si>
+  <si>
+    <t>10:00-11:15</t>
+  </si>
+  <si>
+    <t>10:15-11:15</t>
+  </si>
+  <si>
+    <t>10:30-11:25</t>
+  </si>
+  <si>
+    <t>10:15-11:30</t>
+  </si>
+  <si>
+    <t>10:15-10:45</t>
+  </si>
+  <si>
+    <t>9:45-10:35
+10:45-11:35</t>
+  </si>
+  <si>
+    <t>8:30-9:10</t>
+  </si>
+  <si>
+    <t>10:30-11:30</t>
+  </si>
+  <si>
+    <t>9:45-10:55</t>
+  </si>
+  <si>
+    <t>9:45-10:30</t>
+  </si>
+  <si>
+    <t>10:30-10:55</t>
+  </si>
+  <si>
+    <t>9:45-10:45</t>
+  </si>
+  <si>
+    <t>11:15-11:50</t>
+  </si>
+  <si>
+    <t>8:30-10:45</t>
+  </si>
+  <si>
+    <t>8:30-10:30</t>
+  </si>
+  <si>
+    <t>8:30-11:00</t>
+  </si>
+  <si>
+    <t>8:30-11:30</t>
+  </si>
+  <si>
+    <t>10:30-11:05
+10:40-11:25</t>
+  </si>
+  <si>
+    <t>10:30-11:45</t>
+  </si>
+  <si>
+    <t>10:00-11:30</t>
+  </si>
+  <si>
+    <t>11:15-12:05
+11:25-12:20</t>
+  </si>
+  <si>
+    <t>12:05-13:05
+12:15-13:25</t>
+  </si>
+  <si>
+    <t>12:00-12:30</t>
+  </si>
+  <si>
+    <t>11:30-12:35</t>
+  </si>
+  <si>
+    <t>11:30-12:10
+11:40-12:25</t>
+  </si>
+  <si>
+    <t>11:15-12:30</t>
+  </si>
+  <si>
+    <t>11:00-12:00</t>
+  </si>
+  <si>
+    <t>10:00-12:00</t>
+  </si>
+  <si>
+    <t>8:30-12:30</t>
+  </si>
+  <si>
+    <t>11:00-12:30</t>
+  </si>
+  <si>
+    <t>11:15-12:45</t>
+  </si>
+  <si>
+    <t>10:15-12:45</t>
+  </si>
+  <si>
+    <t>11:00-11:45
+11:10-12:05</t>
+  </si>
+  <si>
+    <t>11:00-13:00</t>
+  </si>
+  <si>
+    <t>10:30-12:15</t>
+  </si>
+  <si>
+    <t>10:15-12:30</t>
+  </si>
+  <si>
+    <t>10:15-11:05
+11:15-12:05</t>
   </si>
 </sst>
 </file>
@@ -1904,6 +1905,24 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1913,24 +1932,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1940,6 +1941,12 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1949,16 +1956,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2244,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="N115" sqref="N115"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="N59" sqref="N59:N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>
@@ -2255,7 +2256,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.6" thickBot="1">
       <c r="A1" s="54" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
@@ -2306,25 +2307,25 @@
         <v>10</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="I3" s="23" t="s">
         <v>15</v>
@@ -2375,7 +2376,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>18</v>
@@ -2399,22 +2400,22 @@
       <c r="D6" s="58"/>
       <c r="E6" s="58"/>
       <c r="F6" s="24" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="42.9" thickBot="1">
@@ -2422,34 +2423,34 @@
         <v>10</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="C7" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.6" thickBot="1">
@@ -2491,7 +2492,7 @@
         <v>18</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>18</v>
@@ -2506,7 +2507,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="57" thickBot="1">
+    <row r="10" spans="1:11" ht="28.75" thickBot="1">
       <c r="A10" s="24" t="s">
         <v>13</v>
       </c>
@@ -2515,22 +2516,22 @@
       <c r="D10" s="58"/>
       <c r="E10" s="58"/>
       <c r="F10" s="24" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>29</v>
+        <v>139</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>27</v>
+        <v>140</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>84</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="28.75" thickBot="1">
@@ -2538,25 +2539,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>165</v>
-      </c>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
+        <v>119</v>
+      </c>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
       <c r="I11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
+        <v>21</v>
+      </c>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:11" ht="14.6" thickBot="1">
       <c r="A12" s="3" t="s">
@@ -2566,14 +2567,14 @@
       <c r="C12" s="58"/>
       <c r="D12" s="58"/>
       <c r="E12" s="58"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
       <c r="I12" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
+        <v>128</v>
+      </c>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
     </row>
     <row r="13" spans="1:11" ht="57" thickBot="1">
       <c r="A13" s="4" t="s">
@@ -2583,14 +2584,14 @@
       <c r="C13" s="58"/>
       <c r="D13" s="58"/>
       <c r="E13" s="58"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
       <c r="I13" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
+        <v>122</v>
+      </c>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
     </row>
     <row r="14" spans="1:11" ht="57" thickBot="1">
       <c r="A14" s="24" t="s">
@@ -2600,18 +2601,18 @@
       <c r="C14" s="58"/>
       <c r="D14" s="58"/>
       <c r="E14" s="58"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
       <c r="I14" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
+        <v>141</v>
+      </c>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
     </row>
     <row r="16" spans="1:11" ht="14.6" thickBot="1">
       <c r="A16" s="9" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.45" thickBot="1">
@@ -2659,42 +2660,42 @@
     </row>
     <row r="18" spans="1:11" ht="30.45" thickBot="1">
       <c r="A18" s="49" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="C18" s="59" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="D18" s="59" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="E18" s="59" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="J18" s="32" t="s">
         <v>15</v>
       </c>
       <c r="K18" s="32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.9" thickBot="1">
       <c r="A19" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -2721,96 +2722,96 @@
     </row>
     <row r="20" spans="1:11" ht="15.9" thickBot="1">
       <c r="A20" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B20" s="59"/>
       <c r="C20" s="59"/>
       <c r="D20" s="59"/>
       <c r="E20" s="59"/>
       <c r="F20" s="12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.9" thickBot="1">
       <c r="A21" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
       <c r="F21" s="50" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="G21" s="50" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="I21" s="50" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="J21" s="50" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="K21" s="50" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30.45" thickBot="1">
       <c r="A22" s="49" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B22" s="55" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="D22" s="55" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.9" thickBot="1">
       <c r="A23" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B23" s="56"/>
       <c r="C23" s="56"/>
@@ -2837,88 +2838,88 @@
     </row>
     <row r="24" spans="1:11" ht="15.9" thickBot="1">
       <c r="A24" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B24" s="56"/>
       <c r="C24" s="56"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
       <c r="F24" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="46.75" thickBot="1">
       <c r="A25" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B25" s="57"/>
       <c r="C25" s="57"/>
       <c r="D25" s="57"/>
       <c r="E25" s="57"/>
       <c r="F25" s="50" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="G25" s="50" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="H25" s="50" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="I25" s="50" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="J25" s="50" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="K25" s="50" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30.45" thickBot="1">
       <c r="A26" s="49" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="C26" s="59" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="D26" s="59" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="E26" s="59" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="F26" s="60"/>
       <c r="G26" s="60"/>
       <c r="H26" s="60"/>
       <c r="I26" s="60"/>
       <c r="J26" s="30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.9" thickBot="1">
       <c r="A27" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B27" s="59"/>
       <c r="C27" s="59"/>
@@ -2929,15 +2930,15 @@
       <c r="H27" s="60"/>
       <c r="I27" s="60"/>
       <c r="J27" s="12" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="46.75" thickBot="1">
       <c r="A28" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B28" s="59"/>
       <c r="C28" s="59"/>
@@ -2948,15 +2949,15 @@
       <c r="H28" s="60"/>
       <c r="I28" s="60"/>
       <c r="J28" s="12" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="62.15" thickBot="1">
       <c r="A29" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B29" s="59"/>
       <c r="C29" s="59"/>
@@ -2967,15 +2968,15 @@
       <c r="H29" s="60"/>
       <c r="I29" s="60"/>
       <c r="J29" s="50" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="K29" s="50" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.9" thickBot="1">
       <c r="A31" s="14" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.45" thickBot="1">
@@ -3023,42 +3024,42 @@
     </row>
     <row r="33" spans="1:11" ht="32.15" thickBot="1">
       <c r="A33" s="49" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="I33" s="34" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="J33" s="35" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="K33" s="35" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.9" thickBot="1">
       <c r="A34" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B34" s="12">
         <v>75</v>
@@ -3093,112 +3094,112 @@
     </row>
     <row r="35" spans="1:11" ht="15.9" thickBot="1">
       <c r="A35" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.9" thickBot="1">
       <c r="A36" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B36" s="50" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="D36" s="50" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="E36" s="50" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="F36" s="50" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="G36" s="50" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
       <c r="H36" s="50" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="I36" s="50" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="J36" s="50" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
       <c r="K36" s="50" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="40.299999999999997" thickBot="1">
       <c r="A37" s="49" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="K37" s="31" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.9" thickBot="1">
       <c r="A38" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B38" s="12">
         <v>75</v>
@@ -3233,92 +3234,92 @@
     </row>
     <row r="39" spans="1:11" ht="15.9" thickBot="1">
       <c r="A39" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="31.3" thickBot="1">
       <c r="A40" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="C40" s="50" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="D40" s="50" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="E40" s="50" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="F40" s="50" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="G40" s="50" t="s">
-        <v>51</v>
+        <v>153</v>
       </c>
       <c r="H40" s="50" t="s">
-        <v>52</v>
+        <v>154</v>
       </c>
       <c r="I40" s="50" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="J40" s="50" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="K40" s="50" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30.45" thickBot="1">
       <c r="A41" s="49" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B41" s="61"/>
       <c r="C41" s="61"/>
       <c r="D41" s="38" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="G41" s="71"/>
       <c r="H41" s="30" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I41" s="71"/>
       <c r="J41" s="71"/>
@@ -3326,7 +3327,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.9" thickBot="1">
       <c r="A42" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B42" s="61"/>
       <c r="C42" s="61"/>
@@ -3341,7 +3342,7 @@
       </c>
       <c r="G42" s="72"/>
       <c r="H42" s="12" t="s">
-        <v>178</v>
+        <v>130</v>
       </c>
       <c r="I42" s="72"/>
       <c r="J42" s="72"/>
@@ -3349,22 +3350,22 @@
     </row>
     <row r="43" spans="1:11" ht="62.15" thickBot="1">
       <c r="A43" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B43" s="61"/>
       <c r="C43" s="61"/>
       <c r="D43" s="12" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G43" s="72"/>
       <c r="H43" s="12" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="I43" s="72"/>
       <c r="J43" s="72"/>
@@ -3372,22 +3373,22 @@
     </row>
     <row r="44" spans="1:11" ht="62.15" thickBot="1">
       <c r="A44" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B44" s="61"/>
       <c r="C44" s="61"/>
       <c r="D44" s="50" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="E44" s="50" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="F44" s="50" t="s">
-        <v>56</v>
+        <v>167</v>
       </c>
       <c r="G44" s="73"/>
       <c r="H44" s="50" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
       <c r="I44" s="73"/>
       <c r="J44" s="73"/>
@@ -3395,7 +3396,7 @@
     </row>
     <row r="46" spans="1:11" ht="15.45" thickBot="1">
       <c r="A46" s="16" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.45" thickBot="1">
@@ -3443,42 +3444,42 @@
     </row>
     <row r="48" spans="1:11" ht="30.45" thickBot="1">
       <c r="A48" s="49" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C48" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G48" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E48" s="30" t="s">
+      <c r="H48" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I48" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="J48" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="42" t="s">
         <v>61</v>
-      </c>
-      <c r="F48" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="G48" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="H48" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="I48" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="J48" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="K48" s="42" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.9" thickBot="1">
       <c r="A49" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B49" s="12">
         <v>135</v>
@@ -3513,111 +3514,111 @@
     </row>
     <row r="50" spans="1:11" ht="28.75" thickBot="1">
       <c r="A50" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="I50" s="18" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="J50" s="18" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="K50" s="18" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.9" thickBot="1">
       <c r="A51" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="C51" s="50" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="E51" s="50" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="F51" s="50" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="G51" s="50" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="H51" s="50" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="I51" s="50" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="J51" s="50" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="K51" s="50" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="30.45" thickBot="1">
       <c r="A52" s="49" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="C52" s="77"/>
+        <v>108</v>
+      </c>
+      <c r="C52" s="74"/>
       <c r="D52" s="30" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="F52" s="39" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="G52" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H52" s="62"/>
+        <v>21</v>
+      </c>
+      <c r="H52" s="68"/>
       <c r="I52" s="43" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="J52" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="K52" s="62"/>
+        <v>53</v>
+      </c>
+      <c r="K52" s="68"/>
     </row>
     <row r="53" spans="1:11" ht="15.9" thickBot="1">
       <c r="A53" s="21" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B53" s="12">
         <v>90</v>
       </c>
-      <c r="C53" s="77"/>
+      <c r="C53" s="74"/>
       <c r="D53" s="13">
         <v>75</v>
       </c>
@@ -3628,494 +3629,494 @@
         <v>120</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="H53" s="63"/>
+        <v>131</v>
+      </c>
+      <c r="H53" s="69"/>
       <c r="I53" s="18">
         <v>90</v>
       </c>
       <c r="J53" s="18">
         <v>120</v>
       </c>
-      <c r="K53" s="63"/>
+      <c r="K53" s="69"/>
     </row>
     <row r="54" spans="1:11" ht="62.15" thickBot="1">
       <c r="A54" s="21" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C54" s="77"/>
+        <v>56</v>
+      </c>
+      <c r="C54" s="74"/>
       <c r="D54" s="15" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="H54" s="63"/>
+        <v>124</v>
+      </c>
+      <c r="H54" s="69"/>
       <c r="I54" s="18" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="J54" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="K54" s="63"/>
-    </row>
-    <row r="55" spans="1:11" ht="62.15" thickBot="1">
+        <v>87</v>
+      </c>
+      <c r="K54" s="69"/>
+    </row>
+    <row r="55" spans="1:11" ht="31.3" thickBot="1">
       <c r="A55" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="77"/>
+        <v>174</v>
+      </c>
+      <c r="C55" s="74"/>
       <c r="D55" s="50" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="E55" s="50" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="F55" s="50" t="s">
-        <v>105</v>
+        <v>171</v>
       </c>
       <c r="G55" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="H55" s="64"/>
+        <v>161</v>
+      </c>
+      <c r="H55" s="70"/>
       <c r="I55" s="50" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="J55" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="K55" s="64"/>
+        <v>158</v>
+      </c>
+      <c r="K55" s="70"/>
     </row>
     <row r="56" spans="1:11" ht="15.9" thickBot="1">
       <c r="A56" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B56" s="62"/>
-      <c r="C56" s="62"/>
-      <c r="D56" s="62"/>
-      <c r="E56" s="62"/>
-      <c r="F56" s="62"/>
-      <c r="G56" s="62"/>
-      <c r="H56" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="68"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="68"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="68"/>
+      <c r="H56" s="68"/>
       <c r="I56" s="44" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J56" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="K56" s="62"/>
+        <v>51</v>
+      </c>
+      <c r="K56" s="68"/>
     </row>
     <row r="57" spans="1:11" ht="15.9" thickBot="1">
       <c r="A57" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B57" s="63"/>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
-      <c r="F57" s="63"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="B57" s="69"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="69"/>
       <c r="I57" s="18">
         <v>135</v>
       </c>
       <c r="J57" s="18">
         <v>150</v>
       </c>
-      <c r="K57" s="63"/>
+      <c r="K57" s="69"/>
     </row>
     <row r="58" spans="1:11" ht="31.3" thickBot="1">
       <c r="A58" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B58" s="63"/>
-      <c r="C58" s="63"/>
-      <c r="D58" s="63"/>
-      <c r="E58" s="63"/>
-      <c r="F58" s="63"/>
-      <c r="G58" s="63"/>
-      <c r="H58" s="63"/>
+        <v>25</v>
+      </c>
+      <c r="B58" s="69"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="69"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="69"/>
       <c r="I58" s="18" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="J58" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="K58" s="63"/>
+        <v>89</v>
+      </c>
+      <c r="K58" s="69"/>
     </row>
     <row r="59" spans="1:11" ht="15.9" thickBot="1">
       <c r="A59" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="64"/>
-      <c r="C59" s="64"/>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
-      <c r="F59" s="64"/>
-      <c r="G59" s="64"/>
-      <c r="H59" s="64"/>
+        <v>27</v>
+      </c>
+      <c r="B59" s="70"/>
+      <c r="C59" s="70"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="70"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="70"/>
       <c r="I59" s="50" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="J59" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="K59" s="64"/>
+        <v>159</v>
+      </c>
+      <c r="K59" s="70"/>
     </row>
     <row r="60" spans="1:11" ht="15.9" thickBot="1">
       <c r="A60" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" s="62"/>
-      <c r="C60" s="62"/>
-      <c r="D60" s="62"/>
-      <c r="E60" s="62"/>
-      <c r="F60" s="62"/>
-      <c r="G60" s="62"/>
-      <c r="H60" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="B60" s="68"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="68"/>
+      <c r="E60" s="68"/>
+      <c r="F60" s="68"/>
+      <c r="G60" s="68"/>
+      <c r="H60" s="68"/>
       <c r="I60" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="J60" s="62"/>
-      <c r="K60" s="62"/>
+        <v>64</v>
+      </c>
+      <c r="J60" s="68"/>
+      <c r="K60" s="68"/>
     </row>
     <row r="61" spans="1:11" ht="15.9" thickBot="1">
       <c r="A61" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" s="63"/>
-      <c r="C61" s="63"/>
-      <c r="D61" s="63"/>
-      <c r="E61" s="63"/>
-      <c r="F61" s="63"/>
-      <c r="G61" s="63"/>
-      <c r="H61" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="B61" s="69"/>
+      <c r="C61" s="69"/>
+      <c r="D61" s="69"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="69"/>
+      <c r="G61" s="69"/>
+      <c r="H61" s="69"/>
       <c r="I61" s="18">
         <v>60</v>
       </c>
-      <c r="J61" s="63"/>
-      <c r="K61" s="63"/>
+      <c r="J61" s="69"/>
+      <c r="K61" s="69"/>
     </row>
     <row r="62" spans="1:11" ht="15.9" thickBot="1">
       <c r="A62" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="63"/>
-      <c r="C62" s="63"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="63"/>
+        <v>25</v>
+      </c>
+      <c r="B62" s="69"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="69"/>
+      <c r="E62" s="69"/>
+      <c r="F62" s="69"/>
+      <c r="G62" s="69"/>
+      <c r="H62" s="69"/>
       <c r="I62" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="J62" s="63"/>
-      <c r="K62" s="63"/>
+        <v>90</v>
+      </c>
+      <c r="J62" s="69"/>
+      <c r="K62" s="69"/>
     </row>
     <row r="63" spans="1:11" ht="15.9" thickBot="1">
       <c r="A63" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B63" s="64"/>
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="64"/>
-      <c r="H63" s="64"/>
+        <v>27</v>
+      </c>
+      <c r="B63" s="70"/>
+      <c r="C63" s="70"/>
+      <c r="D63" s="70"/>
+      <c r="E63" s="70"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
       <c r="I63" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="J63" s="64"/>
-      <c r="K63" s="64"/>
+        <v>133</v>
+      </c>
+      <c r="J63" s="70"/>
+      <c r="K63" s="70"/>
     </row>
     <row r="64" spans="1:11" ht="15.9" thickBot="1">
       <c r="A64" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" s="62"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
-      <c r="E64" s="62"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="B64" s="68"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="68"/>
+      <c r="H64" s="68"/>
       <c r="I64" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="J64" s="62"/>
-      <c r="K64" s="62"/>
+        <v>65</v>
+      </c>
+      <c r="J64" s="68"/>
+      <c r="K64" s="68"/>
     </row>
     <row r="65" spans="1:11" ht="15.9" thickBot="1">
       <c r="A65" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B65" s="63"/>
-      <c r="C65" s="63"/>
-      <c r="D65" s="63"/>
-      <c r="E65" s="63"/>
-      <c r="F65" s="63"/>
-      <c r="G65" s="63"/>
-      <c r="H65" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="B65" s="69"/>
+      <c r="C65" s="69"/>
+      <c r="D65" s="69"/>
+      <c r="E65" s="69"/>
+      <c r="F65" s="69"/>
+      <c r="G65" s="69"/>
+      <c r="H65" s="69"/>
       <c r="I65" s="18">
         <v>120</v>
       </c>
-      <c r="J65" s="63"/>
-      <c r="K65" s="63"/>
+      <c r="J65" s="69"/>
+      <c r="K65" s="69"/>
     </row>
     <row r="66" spans="1:11" ht="15.9" thickBot="1">
       <c r="A66" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B66" s="63"/>
-      <c r="C66" s="63"/>
-      <c r="D66" s="63"/>
-      <c r="E66" s="63"/>
-      <c r="F66" s="63"/>
-      <c r="G66" s="63"/>
-      <c r="H66" s="63"/>
+        <v>25</v>
+      </c>
+      <c r="B66" s="69"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="69"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="69"/>
+      <c r="H66" s="69"/>
       <c r="I66" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="J66" s="63"/>
-      <c r="K66" s="63"/>
+        <v>91</v>
+      </c>
+      <c r="J66" s="69"/>
+      <c r="K66" s="69"/>
     </row>
     <row r="67" spans="1:11" ht="15.9" thickBot="1">
       <c r="A67" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B67" s="64"/>
-      <c r="C67" s="64"/>
-      <c r="D67" s="64"/>
-      <c r="E67" s="64"/>
-      <c r="F67" s="64"/>
-      <c r="G67" s="64"/>
-      <c r="H67" s="64"/>
+        <v>27</v>
+      </c>
+      <c r="B67" s="70"/>
+      <c r="C67" s="70"/>
+      <c r="D67" s="70"/>
+      <c r="E67" s="70"/>
+      <c r="F67" s="70"/>
+      <c r="G67" s="70"/>
+      <c r="H67" s="70"/>
       <c r="I67" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="J67" s="64"/>
-      <c r="K67" s="64"/>
+        <v>158</v>
+      </c>
+      <c r="J67" s="70"/>
+      <c r="K67" s="70"/>
     </row>
     <row r="68" spans="1:11" ht="15.9" thickBot="1">
       <c r="A68" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B68" s="62"/>
-      <c r="C68" s="62"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
-      <c r="G68" s="62"/>
-      <c r="H68" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="B68" s="68"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="68"/>
+      <c r="H68" s="68"/>
       <c r="I68" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="J68" s="62"/>
-      <c r="K68" s="62"/>
+        <v>45</v>
+      </c>
+      <c r="J68" s="68"/>
+      <c r="K68" s="68"/>
     </row>
     <row r="69" spans="1:11" ht="15.9" thickBot="1">
       <c r="A69" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B69" s="63"/>
-      <c r="C69" s="63"/>
-      <c r="D69" s="63"/>
-      <c r="E69" s="63"/>
-      <c r="F69" s="63"/>
-      <c r="G69" s="63"/>
-      <c r="H69" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="B69" s="69"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="69"/>
+      <c r="E69" s="69"/>
+      <c r="F69" s="69"/>
+      <c r="G69" s="69"/>
+      <c r="H69" s="69"/>
       <c r="I69" s="18">
         <v>90</v>
       </c>
-      <c r="J69" s="63"/>
-      <c r="K69" s="63"/>
+      <c r="J69" s="69"/>
+      <c r="K69" s="69"/>
     </row>
     <row r="70" spans="1:11" ht="15.9" thickBot="1">
       <c r="A70" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B70" s="63"/>
-      <c r="C70" s="63"/>
-      <c r="D70" s="63"/>
-      <c r="E70" s="63"/>
-      <c r="F70" s="63"/>
-      <c r="G70" s="63"/>
-      <c r="H70" s="63"/>
+        <v>25</v>
+      </c>
+      <c r="B70" s="69"/>
+      <c r="C70" s="69"/>
+      <c r="D70" s="69"/>
+      <c r="E70" s="69"/>
+      <c r="F70" s="69"/>
+      <c r="G70" s="69"/>
+      <c r="H70" s="69"/>
       <c r="I70" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="J70" s="63"/>
-      <c r="K70" s="63"/>
+        <v>92</v>
+      </c>
+      <c r="J70" s="69"/>
+      <c r="K70" s="69"/>
     </row>
     <row r="71" spans="1:11" ht="15.9" thickBot="1">
       <c r="A71" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B71" s="64"/>
-      <c r="C71" s="64"/>
-      <c r="D71" s="64"/>
-      <c r="E71" s="64"/>
-      <c r="F71" s="64"/>
-      <c r="G71" s="64"/>
-      <c r="H71" s="64"/>
+        <v>27</v>
+      </c>
+      <c r="B71" s="70"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="70"/>
+      <c r="E71" s="70"/>
+      <c r="F71" s="70"/>
+      <c r="G71" s="70"/>
+      <c r="H71" s="70"/>
       <c r="I71" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="J71" s="64"/>
-      <c r="K71" s="64"/>
+        <v>135</v>
+      </c>
+      <c r="J71" s="70"/>
+      <c r="K71" s="70"/>
     </row>
     <row r="72" spans="1:11" ht="15.9" thickBot="1">
       <c r="A72" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B72" s="62"/>
-      <c r="C72" s="62"/>
-      <c r="D72" s="62"/>
-      <c r="E72" s="62"/>
-      <c r="F72" s="62"/>
-      <c r="G72" s="62"/>
-      <c r="H72" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="B72" s="68"/>
+      <c r="C72" s="68"/>
+      <c r="D72" s="68"/>
+      <c r="E72" s="68"/>
+      <c r="F72" s="68"/>
+      <c r="G72" s="68"/>
+      <c r="H72" s="68"/>
       <c r="I72" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="J72" s="62"/>
-      <c r="K72" s="62"/>
+        <v>69</v>
+      </c>
+      <c r="J72" s="68"/>
+      <c r="K72" s="68"/>
     </row>
     <row r="73" spans="1:11" ht="15.9" thickBot="1">
       <c r="A73" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B73" s="63"/>
-      <c r="C73" s="63"/>
-      <c r="D73" s="63"/>
-      <c r="E73" s="63"/>
-      <c r="F73" s="63"/>
-      <c r="G73" s="63"/>
-      <c r="H73" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="B73" s="69"/>
+      <c r="C73" s="69"/>
+      <c r="D73" s="69"/>
+      <c r="E73" s="69"/>
+      <c r="F73" s="69"/>
+      <c r="G73" s="69"/>
+      <c r="H73" s="69"/>
       <c r="I73" s="18">
         <v>75</v>
       </c>
-      <c r="J73" s="63"/>
-      <c r="K73" s="63"/>
+      <c r="J73" s="69"/>
+      <c r="K73" s="69"/>
     </row>
     <row r="74" spans="1:11" ht="15.9" thickBot="1">
       <c r="A74" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B74" s="63"/>
-      <c r="C74" s="63"/>
-      <c r="D74" s="63"/>
-      <c r="E74" s="63"/>
-      <c r="F74" s="63"/>
-      <c r="G74" s="63"/>
-      <c r="H74" s="63"/>
+        <v>25</v>
+      </c>
+      <c r="B74" s="69"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="69"/>
+      <c r="F74" s="69"/>
+      <c r="G74" s="69"/>
+      <c r="H74" s="69"/>
       <c r="I74" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="J74" s="63"/>
-      <c r="K74" s="63"/>
+        <v>86</v>
+      </c>
+      <c r="J74" s="69"/>
+      <c r="K74" s="69"/>
     </row>
     <row r="75" spans="1:11" ht="31.3" thickBot="1">
       <c r="A75" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B75" s="64"/>
-      <c r="C75" s="64"/>
-      <c r="D75" s="64"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="64"/>
-      <c r="G75" s="64"/>
-      <c r="H75" s="64"/>
+        <v>27</v>
+      </c>
+      <c r="B75" s="70"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="70"/>
+      <c r="F75" s="70"/>
+      <c r="G75" s="70"/>
+      <c r="H75" s="70"/>
       <c r="I75" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="J75" s="64"/>
-      <c r="K75" s="64"/>
+        <v>162</v>
+      </c>
+      <c r="J75" s="70"/>
+      <c r="K75" s="70"/>
     </row>
     <row r="76" spans="1:11" ht="15.9" thickBot="1">
       <c r="A76" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="B76" s="62"/>
-      <c r="C76" s="78"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="62"/>
-      <c r="F76" s="62"/>
-      <c r="G76" s="62"/>
-      <c r="H76" s="79"/>
+        <v>23</v>
+      </c>
+      <c r="B76" s="68"/>
+      <c r="C76" s="75"/>
+      <c r="D76" s="76"/>
+      <c r="E76" s="68"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="68"/>
+      <c r="H76" s="80"/>
       <c r="I76" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="J76" s="77"/>
-      <c r="K76" s="77"/>
+        <v>70</v>
+      </c>
+      <c r="J76" s="74"/>
+      <c r="K76" s="74"/>
     </row>
     <row r="77" spans="1:11" ht="15.9" thickBot="1">
       <c r="A77" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B77" s="63"/>
-      <c r="C77" s="78"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="63"/>
-      <c r="F77" s="63"/>
-      <c r="G77" s="63"/>
-      <c r="H77" s="79"/>
+        <v>24</v>
+      </c>
+      <c r="B77" s="69"/>
+      <c r="C77" s="75"/>
+      <c r="D77" s="77"/>
+      <c r="E77" s="69"/>
+      <c r="F77" s="69"/>
+      <c r="G77" s="69"/>
+      <c r="H77" s="80"/>
       <c r="I77" s="18">
         <v>90</v>
       </c>
-      <c r="J77" s="77"/>
-      <c r="K77" s="77"/>
+      <c r="J77" s="74"/>
+      <c r="K77" s="74"/>
     </row>
     <row r="78" spans="1:11" ht="15.9" thickBot="1">
       <c r="A78" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B78" s="63"/>
-      <c r="C78" s="78"/>
-      <c r="D78" s="75"/>
-      <c r="E78" s="63"/>
-      <c r="F78" s="63"/>
-      <c r="G78" s="63"/>
-      <c r="H78" s="79"/>
+        <v>25</v>
+      </c>
+      <c r="B78" s="69"/>
+      <c r="C78" s="75"/>
+      <c r="D78" s="77"/>
+      <c r="E78" s="69"/>
+      <c r="F78" s="69"/>
+      <c r="G78" s="69"/>
+      <c r="H78" s="80"/>
       <c r="I78" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="J78" s="77"/>
-      <c r="K78" s="77"/>
+        <v>90</v>
+      </c>
+      <c r="J78" s="74"/>
+      <c r="K78" s="74"/>
     </row>
     <row r="79" spans="1:11" ht="31.3" thickBot="1">
       <c r="A79" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B79" s="64"/>
-      <c r="C79" s="78"/>
-      <c r="D79" s="76"/>
-      <c r="E79" s="64"/>
-      <c r="F79" s="64"/>
-      <c r="G79" s="64"/>
-      <c r="H79" s="79"/>
+        <v>27</v>
+      </c>
+      <c r="B79" s="70"/>
+      <c r="C79" s="75"/>
+      <c r="D79" s="78"/>
+      <c r="E79" s="70"/>
+      <c r="F79" s="70"/>
+      <c r="G79" s="70"/>
+      <c r="H79" s="80"/>
       <c r="I79" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="J79" s="77"/>
-      <c r="K79" s="77"/>
+        <v>163</v>
+      </c>
+      <c r="J79" s="74"/>
+      <c r="K79" s="74"/>
     </row>
     <row r="81" spans="1:11" ht="14.6" thickBot="1">
       <c r="A81" s="19" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.45" thickBot="1">
@@ -4163,42 +4164,42 @@
     </row>
     <row r="83" spans="1:11" ht="30.45" thickBot="1">
       <c r="A83" s="49" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B83" s="30" t="s">
         <v>14</v>
       </c>
       <c r="C83" s="42" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="D83" s="42" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="E83" s="51" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="F83" s="30" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="G83" s="52" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H83" s="38" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="I83" s="36" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="J83" s="51" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="K83" s="42" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15.45">
       <c r="A84" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B84" s="12">
         <v>120</v>
@@ -4233,110 +4234,110 @@
     </row>
     <row r="85" spans="1:11" ht="31.3" thickBot="1">
       <c r="A85" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="J85" s="13" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="K85" s="18" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="15.9" thickBot="1">
       <c r="A86" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B86" s="50" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="C86" s="50" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="D86" s="50" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="E86" s="50" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="F86" s="50" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="G86" s="50" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="H86" s="50" t="s">
-        <v>114</v>
+        <v>172</v>
       </c>
       <c r="I86" s="50" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="J86" s="50" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="K86" s="50" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="30.45" thickBot="1">
       <c r="A87" s="49" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="C87" s="39" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="D87" s="39" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="E87" s="31" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="F87" s="43" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G87" s="30" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="H87" s="31" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="I87" s="41" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="J87" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="K87" s="62"/>
+        <v>81</v>
+      </c>
+      <c r="K87" s="68"/>
     </row>
     <row r="88" spans="1:11" ht="15.9" thickBot="1">
       <c r="A88" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B88" s="12">
         <v>90</v>
@@ -4351,7 +4352,7 @@
         <v>150</v>
       </c>
       <c r="F88" s="20" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="G88" s="12">
         <v>90</v>
@@ -4365,104 +4366,104 @@
       <c r="J88" s="12">
         <v>120</v>
       </c>
-      <c r="K88" s="63"/>
+      <c r="K88" s="69"/>
     </row>
     <row r="89" spans="1:11" ht="62.15" thickBot="1">
       <c r="A89" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="F89" s="18" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="G89" s="12" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="I89" s="18" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
       <c r="J89" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="K89" s="63"/>
+        <v>103</v>
+      </c>
+      <c r="K89" s="69"/>
     </row>
     <row r="90" spans="1:11" ht="62.15" thickBot="1">
       <c r="A90" s="50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B90" s="50" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="C90" s="50" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="D90" s="50" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="E90" s="50" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="F90" s="50" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="G90" s="50" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="H90" s="50" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="I90" s="50" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="J90" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="K90" s="64"/>
+        <v>171</v>
+      </c>
+      <c r="K90" s="70"/>
     </row>
     <row r="91" spans="1:11" ht="15.9" thickBot="1">
       <c r="A91" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B91" s="62"/>
-      <c r="C91" s="62"/>
-      <c r="D91" s="62"/>
-      <c r="E91" s="62"/>
-      <c r="F91" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="B91" s="68"/>
+      <c r="C91" s="68"/>
+      <c r="D91" s="68"/>
+      <c r="E91" s="68"/>
+      <c r="F91" s="68"/>
       <c r="G91" s="51" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="H91" s="51" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="I91" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="J91" s="62"/>
-      <c r="K91" s="62"/>
+        <v>82</v>
+      </c>
+      <c r="J91" s="68"/>
+      <c r="K91" s="68"/>
     </row>
     <row r="92" spans="1:11" ht="15.9" thickBot="1">
       <c r="A92" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B92" s="63"/>
-      <c r="C92" s="63"/>
-      <c r="D92" s="63"/>
-      <c r="E92" s="63"/>
-      <c r="F92" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="B92" s="69"/>
+      <c r="C92" s="69"/>
+      <c r="D92" s="69"/>
+      <c r="E92" s="69"/>
+      <c r="F92" s="69"/>
       <c r="G92" s="12">
         <v>75</v>
       </c>
@@ -4472,257 +4473,259 @@
       <c r="I92" s="12">
         <v>120</v>
       </c>
-      <c r="J92" s="63"/>
-      <c r="K92" s="63"/>
+      <c r="J92" s="69"/>
+      <c r="K92" s="69"/>
     </row>
     <row r="93" spans="1:11" ht="15.9" thickBot="1">
       <c r="A93" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B93" s="63"/>
-      <c r="C93" s="63"/>
-      <c r="D93" s="63"/>
-      <c r="E93" s="63"/>
-      <c r="F93" s="63"/>
+        <v>25</v>
+      </c>
+      <c r="B93" s="69"/>
+      <c r="C93" s="69"/>
+      <c r="D93" s="69"/>
+      <c r="E93" s="69"/>
+      <c r="F93" s="69"/>
       <c r="G93" s="13" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="H93" s="53" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="J93" s="63"/>
-      <c r="K93" s="63"/>
-    </row>
-    <row r="94" spans="1:11" ht="15.9" thickBot="1">
+        <v>102</v>
+      </c>
+      <c r="J93" s="69"/>
+      <c r="K93" s="69"/>
+    </row>
+    <row r="94" spans="1:11" ht="31.3" thickBot="1">
       <c r="A94" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B94" s="64"/>
-      <c r="C94" s="64"/>
-      <c r="D94" s="64"/>
-      <c r="E94" s="64"/>
-      <c r="F94" s="64"/>
+        <v>27</v>
+      </c>
+      <c r="B94" s="70"/>
+      <c r="C94" s="70"/>
+      <c r="D94" s="70"/>
+      <c r="E94" s="70"/>
+      <c r="F94" s="70"/>
       <c r="G94" s="50" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="H94" s="50" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="I94" s="50" t="s">
-        <v>168</v>
-      </c>
-      <c r="J94" s="64"/>
-      <c r="K94" s="64"/>
+        <v>177</v>
+      </c>
+      <c r="J94" s="70"/>
+      <c r="K94" s="70"/>
     </row>
     <row r="95" spans="1:11" ht="15.9" thickBot="1">
       <c r="A95" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B95" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="B95" s="68"/>
       <c r="C95" s="45"/>
-      <c r="D95" s="62"/>
-      <c r="E95" s="62"/>
-      <c r="F95" s="62"/>
+      <c r="D95" s="68"/>
+      <c r="E95" s="68"/>
+      <c r="F95" s="68"/>
       <c r="G95" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="H95" s="77"/>
-      <c r="I95" s="62"/>
-      <c r="J95" s="62"/>
-      <c r="K95" s="62"/>
+        <v>45</v>
+      </c>
+      <c r="H95" s="74"/>
+      <c r="I95" s="68"/>
+      <c r="J95" s="68"/>
+      <c r="K95" s="68"/>
     </row>
     <row r="96" spans="1:11" ht="15.9" thickBot="1">
       <c r="A96" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B96" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="B96" s="69"/>
       <c r="C96" s="46"/>
-      <c r="D96" s="63"/>
-      <c r="E96" s="63"/>
-      <c r="F96" s="63"/>
+      <c r="D96" s="69"/>
+      <c r="E96" s="69"/>
+      <c r="F96" s="69"/>
       <c r="G96" s="12">
         <v>150</v>
       </c>
-      <c r="H96" s="77"/>
-      <c r="I96" s="63"/>
-      <c r="J96" s="63"/>
-      <c r="K96" s="63"/>
+      <c r="H96" s="74"/>
+      <c r="I96" s="69"/>
+      <c r="J96" s="69"/>
+      <c r="K96" s="69"/>
     </row>
     <row r="97" spans="1:11" ht="15.9" thickBot="1">
       <c r="A97" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B97" s="63"/>
+        <v>25</v>
+      </c>
+      <c r="B97" s="69"/>
       <c r="C97" s="46"/>
-      <c r="D97" s="63"/>
-      <c r="E97" s="63"/>
-      <c r="F97" s="63"/>
+      <c r="D97" s="69"/>
+      <c r="E97" s="69"/>
+      <c r="F97" s="69"/>
       <c r="G97" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="H97" s="77"/>
-      <c r="I97" s="63"/>
-      <c r="J97" s="63"/>
-      <c r="K97" s="63"/>
+        <v>78</v>
+      </c>
+      <c r="H97" s="74"/>
+      <c r="I97" s="69"/>
+      <c r="J97" s="69"/>
+      <c r="K97" s="69"/>
     </row>
     <row r="98" spans="1:11" ht="15.9" thickBot="1">
       <c r="A98" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B98" s="64"/>
+        <v>27</v>
+      </c>
+      <c r="B98" s="70"/>
       <c r="C98" s="47"/>
-      <c r="D98" s="64"/>
-      <c r="E98" s="64"/>
-      <c r="F98" s="64"/>
+      <c r="D98" s="70"/>
+      <c r="E98" s="70"/>
+      <c r="F98" s="70"/>
       <c r="G98" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="H98" s="77"/>
-      <c r="I98" s="64"/>
-      <c r="J98" s="64"/>
-      <c r="K98" s="64"/>
+        <v>159</v>
+      </c>
+      <c r="H98" s="74"/>
+      <c r="I98" s="70"/>
+      <c r="J98" s="70"/>
+      <c r="K98" s="70"/>
     </row>
     <row r="99" spans="1:11" ht="15.9" thickBot="1">
       <c r="A99" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B99" s="62"/>
-      <c r="C99" s="62"/>
-      <c r="D99" s="62"/>
-      <c r="E99" s="62"/>
-      <c r="F99" s="62"/>
+        <v>55</v>
+      </c>
+      <c r="B99" s="68"/>
+      <c r="C99" s="68"/>
+      <c r="D99" s="68"/>
+      <c r="E99" s="68"/>
+      <c r="F99" s="68"/>
       <c r="G99" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="H99" s="80"/>
-      <c r="I99" s="62"/>
-      <c r="J99" s="62"/>
-      <c r="K99" s="80"/>
+        <v>83</v>
+      </c>
+      <c r="H99" s="79"/>
+      <c r="I99" s="68"/>
+      <c r="J99" s="68"/>
+      <c r="K99" s="79"/>
     </row>
     <row r="100" spans="1:11" ht="15.9" thickBot="1">
       <c r="A100" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B100" s="63"/>
-      <c r="C100" s="63"/>
-      <c r="D100" s="63"/>
-      <c r="E100" s="63"/>
-      <c r="F100" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="B100" s="69"/>
+      <c r="C100" s="69"/>
+      <c r="D100" s="69"/>
+      <c r="E100" s="69"/>
+      <c r="F100" s="69"/>
       <c r="G100" s="12">
         <v>105</v>
       </c>
-      <c r="H100" s="80"/>
-      <c r="I100" s="63"/>
-      <c r="J100" s="63"/>
-      <c r="K100" s="80"/>
+      <c r="H100" s="79"/>
+      <c r="I100" s="69"/>
+      <c r="J100" s="69"/>
+      <c r="K100" s="79"/>
     </row>
     <row r="101" spans="1:11" ht="15.9" thickBot="1">
       <c r="A101" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B101" s="63"/>
-      <c r="C101" s="63"/>
-      <c r="D101" s="63"/>
-      <c r="E101" s="63"/>
-      <c r="F101" s="63"/>
+        <v>25</v>
+      </c>
+      <c r="B101" s="69"/>
+      <c r="C101" s="69"/>
+      <c r="D101" s="69"/>
+      <c r="E101" s="69"/>
+      <c r="F101" s="69"/>
       <c r="G101" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="H101" s="80"/>
-      <c r="I101" s="63"/>
-      <c r="J101" s="63"/>
-      <c r="K101" s="80"/>
+        <v>97</v>
+      </c>
+      <c r="H101" s="79"/>
+      <c r="I101" s="69"/>
+      <c r="J101" s="69"/>
+      <c r="K101" s="79"/>
     </row>
     <row r="102" spans="1:11" ht="31.3" thickBot="1">
       <c r="A102" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B102" s="64"/>
-      <c r="C102" s="64"/>
-      <c r="D102" s="64"/>
-      <c r="E102" s="64"/>
-      <c r="F102" s="64"/>
+        <v>27</v>
+      </c>
+      <c r="B102" s="70"/>
+      <c r="C102" s="70"/>
+      <c r="D102" s="70"/>
+      <c r="E102" s="70"/>
+      <c r="F102" s="70"/>
       <c r="G102" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="H102" s="80"/>
-      <c r="I102" s="64"/>
-      <c r="J102" s="64"/>
-      <c r="K102" s="80"/>
+        <v>178</v>
+      </c>
+      <c r="H102" s="79"/>
+      <c r="I102" s="70"/>
+      <c r="J102" s="70"/>
+      <c r="K102" s="79"/>
     </row>
     <row r="103" spans="1:11" ht="15.9" thickBot="1">
       <c r="A103" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B103" s="77"/>
-      <c r="C103" s="77"/>
-      <c r="D103" s="77"/>
-      <c r="E103" s="77"/>
-      <c r="F103" s="77"/>
+        <v>55</v>
+      </c>
+      <c r="B103" s="74"/>
+      <c r="C103" s="74"/>
+      <c r="D103" s="74"/>
+      <c r="E103" s="74"/>
+      <c r="F103" s="74"/>
       <c r="G103" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="H103" s="77"/>
-      <c r="I103" s="77"/>
-      <c r="J103" s="77"/>
-      <c r="K103" s="77"/>
+        <v>70</v>
+      </c>
+      <c r="H103" s="74"/>
+      <c r="I103" s="74"/>
+      <c r="J103" s="74"/>
+      <c r="K103" s="74"/>
     </row>
     <row r="104" spans="1:11" ht="15.9" thickBot="1">
       <c r="A104" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B104" s="77"/>
-      <c r="C104" s="77"/>
-      <c r="D104" s="77"/>
-      <c r="E104" s="77"/>
-      <c r="F104" s="77"/>
+        <v>24</v>
+      </c>
+      <c r="B104" s="74"/>
+      <c r="C104" s="74"/>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="74"/>
       <c r="G104" s="12">
         <v>135</v>
       </c>
-      <c r="H104" s="77"/>
-      <c r="I104" s="77"/>
-      <c r="J104" s="77"/>
-      <c r="K104" s="77"/>
+      <c r="H104" s="74"/>
+      <c r="I104" s="74"/>
+      <c r="J104" s="74"/>
+      <c r="K104" s="74"/>
     </row>
     <row r="105" spans="1:11" ht="15.9" thickBot="1">
       <c r="A105" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B105" s="77"/>
-      <c r="C105" s="77"/>
-      <c r="D105" s="77"/>
-      <c r="E105" s="77"/>
-      <c r="F105" s="77"/>
+        <v>25</v>
+      </c>
+      <c r="B105" s="74"/>
+      <c r="C105" s="74"/>
+      <c r="D105" s="74"/>
+      <c r="E105" s="74"/>
+      <c r="F105" s="74"/>
       <c r="G105" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="H105" s="77"/>
-      <c r="I105" s="77"/>
-      <c r="J105" s="77"/>
-      <c r="K105" s="77"/>
+        <v>98</v>
+      </c>
+      <c r="H105" s="74"/>
+      <c r="I105" s="74"/>
+      <c r="J105" s="74"/>
+      <c r="K105" s="74"/>
     </row>
     <row r="106" spans="1:11" ht="31.3" thickBot="1">
       <c r="A106" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B106" s="77"/>
-      <c r="C106" s="77"/>
-      <c r="D106" s="77"/>
-      <c r="E106" s="77"/>
-      <c r="F106" s="77"/>
+        <v>27</v>
+      </c>
+      <c r="B106" s="74"/>
+      <c r="C106" s="74"/>
+      <c r="D106" s="74"/>
+      <c r="E106" s="74"/>
+      <c r="F106" s="74"/>
       <c r="G106" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="H106" s="77"/>
-      <c r="I106" s="77"/>
-      <c r="J106" s="77"/>
-      <c r="K106" s="77"/>
+        <v>179</v>
+      </c>
+      <c r="H106" s="74"/>
+      <c r="I106" s="74"/>
+      <c r="J106" s="74"/>
+      <c r="K106" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="129">
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="H64:H67"/>
     <mergeCell ref="K87:K90"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="J91:J94"/>
@@ -4733,21 +4736,21 @@
     <mergeCell ref="H103:H106"/>
     <mergeCell ref="I103:I106"/>
     <mergeCell ref="J103:J106"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="G64:G67"/>
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="H64:H67"/>
     <mergeCell ref="H76:H79"/>
     <mergeCell ref="J76:J79"/>
     <mergeCell ref="K76:K79"/>
     <mergeCell ref="J95:J98"/>
     <mergeCell ref="H95:H98"/>
     <mergeCell ref="I95:I98"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K95:K98"/>
+    <mergeCell ref="K99:K102"/>
+    <mergeCell ref="H99:H102"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="D91:D94"/>
+    <mergeCell ref="E91:E94"/>
+    <mergeCell ref="F91:F94"/>
     <mergeCell ref="B103:B106"/>
     <mergeCell ref="C103:C106"/>
     <mergeCell ref="B95:B98"/>
@@ -4757,22 +4760,6 @@
     <mergeCell ref="D103:D106"/>
     <mergeCell ref="E103:E106"/>
     <mergeCell ref="F103:F106"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="C99:C102"/>
-    <mergeCell ref="D99:D102"/>
-    <mergeCell ref="E99:E102"/>
-    <mergeCell ref="F99:F102"/>
-    <mergeCell ref="K95:K98"/>
-    <mergeCell ref="K99:K102"/>
-    <mergeCell ref="H99:H102"/>
-    <mergeCell ref="C91:C94"/>
-    <mergeCell ref="D91:D94"/>
-    <mergeCell ref="E91:E94"/>
-    <mergeCell ref="F91:F94"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="G72:G75"/>
     <mergeCell ref="E76:E79"/>
     <mergeCell ref="F76:F79"/>
     <mergeCell ref="G76:G79"/>
@@ -4780,7 +4767,12 @@
     <mergeCell ref="C76:C79"/>
     <mergeCell ref="B76:B79"/>
     <mergeCell ref="D76:D79"/>
-    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="C99:C102"/>
+    <mergeCell ref="D99:D102"/>
+    <mergeCell ref="E99:E102"/>
+    <mergeCell ref="F99:F102"/>
     <mergeCell ref="C52:C55"/>
     <mergeCell ref="B56:B59"/>
     <mergeCell ref="C56:C59"/>
@@ -4794,7 +4786,6 @@
     <mergeCell ref="E60:E63"/>
     <mergeCell ref="F60:F63"/>
     <mergeCell ref="G60:G63"/>
-    <mergeCell ref="J72:J75"/>
     <mergeCell ref="B64:B67"/>
     <mergeCell ref="B68:B71"/>
     <mergeCell ref="B72:B75"/>
@@ -4804,6 +4795,21 @@
     <mergeCell ref="J60:J63"/>
     <mergeCell ref="K60:K63"/>
     <mergeCell ref="D72:D75"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="G64:G67"/>
     <mergeCell ref="K11:K14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="G11:G14"/>
@@ -4817,11 +4823,6 @@
     <mergeCell ref="J41:J44"/>
     <mergeCell ref="K41:K44"/>
     <mergeCell ref="G41:G44"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="D26:D29"/>

</xml_diff>

<commit_message>
modified:   Input/Exam Timetable.xlsx 	modified:   main.ipynb
</commit_message>
<xml_diff>
--- a/Input/Exam Timetable.xlsx
+++ b/Input/Exam Timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EC6EC9-2DAB-441E-9120-1EDBAD6CAC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784116AA-FA40-4B87-A0F2-F30B7D0E36C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4131" yWindow="9154" windowWidth="24891" windowHeight="15035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -168,9 +168,6 @@
     </r>
   </si>
   <si>
-    <t>04/11/2021 (四)</t>
-  </si>
-  <si>
     <t>09/11/2021 (二)</t>
   </si>
   <si>
@@ -691,6 +688,9 @@
   </si>
   <si>
     <t>10:30am – 11:25am</t>
+  </si>
+  <si>
+    <t>04/11/2021 (四)</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1241,25 +1241,25 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -1267,25 +1267,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1316,16 +1316,16 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1336,16 +1336,16 @@
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -1353,25 +1353,25 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1402,19 +1402,19 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1422,16 +1422,16 @@
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="H10" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1439,16 +1439,16 @@
         <v>0</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
@@ -1476,7 +1476,7 @@
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -1490,7 +1490,7 @@
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -1554,25 +1554,25 @@
         <v>10</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1603,16 +1603,16 @@
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1623,16 +1623,16 @@
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -1640,25 +1640,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1689,16 +1689,16 @@
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -1709,16 +1709,16 @@
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1726,16 +1726,16 @@
         <v>10</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -1763,7 +1763,7 @@
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -1777,7 +1777,7 @@
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
       <c r="E29" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -1841,23 +1841,23 @@
         <v>10</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G33" s="19"/>
       <c r="H33" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1889,23 +1889,23 @@
         <v>12</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1913,23 +1913,23 @@
         <v>9</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="E36" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G36" s="21"/>
       <c r="H36" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1937,23 +1937,23 @@
         <v>10</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="G37" s="19"/>
       <c r="H37" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1985,23 +1985,23 @@
         <v>12</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2009,23 +2009,23 @@
         <v>9</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="E40" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G40" s="21"/>
       <c r="H40" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2039,7 +2039,7 @@
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
       <c r="H41" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2067,7 +2067,7 @@
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
       <c r="H43" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2081,7 +2081,7 @@
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
       <c r="H44" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2106,7 +2106,7 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="11" t="str">
         <f t="shared" ref="B47:H47" si="2">B2</f>
@@ -2142,25 +2142,25 @@
         <v>13</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="F48" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G48" s="5" t="s">
+      <c r="H48" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2194,25 +2194,25 @@
         <v>12</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F50" s="6" t="s">
+      <c r="G50" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G50" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="H50" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2220,25 +2220,25 @@
         <v>9</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F51" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="G51" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="H51" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2246,25 +2246,25 @@
         <v>13</v>
       </c>
       <c r="B52" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="D52" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="F52" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2298,25 +2298,25 @@
         <v>12</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C54" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="E54" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E54" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="F54" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="H54" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2324,25 +2324,25 @@
         <v>9</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2353,13 +2353,13 @@
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F56" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="H56" s="19"/>
     </row>
@@ -2389,13 +2389,13 @@
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
       <c r="E58" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F58" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G58" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="H58" s="20"/>
     </row>
@@ -2407,13 +2407,13 @@
       <c r="C59" s="21"/>
       <c r="D59" s="21"/>
       <c r="E59" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H59" s="21"/>
     </row>
@@ -2426,7 +2426,7 @@
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
       <c r="F60" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="19"/>
@@ -2454,7 +2454,7 @@
       <c r="D62" s="20"/>
       <c r="E62" s="20"/>
       <c r="F62" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
@@ -2468,7 +2468,7 @@
       <c r="D63" s="21"/>
       <c r="E63" s="21"/>
       <c r="F63" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G63" s="21"/>
       <c r="H63" s="21"/>
@@ -2495,7 +2495,7 @@
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
     </row>
-    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="11" t="str">
         <f t="shared" ref="B66:H66" si="3">B2</f>
@@ -2531,25 +2531,25 @@
         <v>13</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="D67" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E67" s="5" t="s">
+      <c r="F67" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="G67" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G67" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="H67" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2583,25 +2583,25 @@
         <v>12</v>
       </c>
       <c r="B69" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D69" s="6" t="s">
+      <c r="E69" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H69" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2609,25 +2609,25 @@
         <v>9</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2635,23 +2635,23 @@
         <v>13</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2683,23 +2683,23 @@
         <v>12</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C73" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="G73" s="18"/>
       <c r="H73" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2707,23 +2707,23 @@
         <v>9</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2733,13 +2733,13 @@
       <c r="B75" s="18"/>
       <c r="C75" s="18"/>
       <c r="D75" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E75" s="18"/>
       <c r="F75" s="18"/>
       <c r="G75" s="18"/>
       <c r="H75" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2765,13 +2765,13 @@
       <c r="B77" s="18"/>
       <c r="C77" s="18"/>
       <c r="D77" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E77" s="18"/>
       <c r="F77" s="18"/>
       <c r="G77" s="18"/>
       <c r="H77" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2781,13 +2781,13 @@
       <c r="B78" s="18"/>
       <c r="C78" s="18"/>
       <c r="D78" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E78" s="18"/>
       <c r="F78" s="18"/>
       <c r="G78" s="18"/>
       <c r="H78" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2797,13 +2797,13 @@
       <c r="B79" s="18"/>
       <c r="C79" s="18"/>
       <c r="D79" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E79" s="18"/>
       <c r="F79" s="18"/>
       <c r="G79" s="18"/>
       <c r="H79" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2829,13 +2829,13 @@
       <c r="B81" s="18"/>
       <c r="C81" s="18"/>
       <c r="D81" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E81" s="18"/>
       <c r="F81" s="18"/>
       <c r="G81" s="18"/>
       <c r="H81" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2845,13 +2845,13 @@
       <c r="B82" s="18"/>
       <c r="C82" s="18"/>
       <c r="D82" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E82" s="18"/>
       <c r="F82" s="18"/>
       <c r="G82" s="18"/>
       <c r="H82" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2861,13 +2861,13 @@
       <c r="B83" s="18"/>
       <c r="C83" s="18"/>
       <c r="D83" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E83" s="18"/>
       <c r="F83" s="18"/>
       <c r="G83" s="18"/>
       <c r="H83" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2893,13 +2893,13 @@
       <c r="B85" s="18"/>
       <c r="C85" s="18"/>
       <c r="D85" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E85" s="18"/>
       <c r="F85" s="18"/>
       <c r="G85" s="18"/>
       <c r="H85" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2909,13 +2909,13 @@
       <c r="B86" s="18"/>
       <c r="C86" s="18"/>
       <c r="D86" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E86" s="18"/>
       <c r="F86" s="18"/>
       <c r="G86" s="18"/>
       <c r="H86" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2925,7 +2925,7 @@
       <c r="B87" s="18"/>
       <c r="C87" s="18"/>
       <c r="D87" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E87" s="18"/>
       <c r="F87" s="18"/>
@@ -2953,7 +2953,7 @@
       <c r="B89" s="18"/>
       <c r="C89" s="18"/>
       <c r="D89" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E89" s="18"/>
       <c r="F89" s="18"/>
@@ -2967,7 +2967,7 @@
       <c r="B90" s="18"/>
       <c r="C90" s="18"/>
       <c r="D90" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
@@ -2996,7 +2996,7 @@
       <c r="G92" s="15"/>
       <c r="H92" s="15"/>
     </row>
-    <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="11" t="str">
         <f t="shared" ref="B93:H93" si="4">B2</f>
@@ -3032,25 +3032,25 @@
         <v>13</v>
       </c>
       <c r="B94" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C94" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="D94" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="E94" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="F94" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="G94" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H94" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="G94" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -3084,25 +3084,25 @@
         <v>12</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E96" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G96" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="F96" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G96" s="6" t="s">
-        <v>168</v>
-      </c>
       <c r="H96" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -3110,25 +3110,25 @@
         <v>9</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E97" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H97" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G97" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="H97" s="7" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -3136,25 +3136,25 @@
         <v>13</v>
       </c>
       <c r="B98" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C98" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="D98" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>148</v>
-      </c>
       <c r="E98" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -3188,25 +3188,25 @@
         <v>12</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F100" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G100" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H100" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="G100" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H100" s="6" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -3214,25 +3214,25 @@
         <v>9</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C101" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D101" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D101" s="7" t="s">
-        <v>170</v>
-      </c>
       <c r="E101" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -3243,11 +3243,11 @@
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F102" s="5"/>
       <c r="G102" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H102" s="5"/>
     </row>
@@ -3275,11 +3275,11 @@
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H104" s="6"/>
     </row>
@@ -3291,11 +3291,11 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H105" s="7"/>
     </row>
@@ -3307,11 +3307,11 @@
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
       <c r="E106" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F106" s="5"/>
       <c r="G106" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H106" s="5"/>
     </row>
@@ -3339,11 +3339,11 @@
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H108" s="6"/>
     </row>
@@ -3355,11 +3355,11 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H109" s="7"/>
     </row>
@@ -3371,11 +3371,11 @@
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F110" s="5"/>
       <c r="G110" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H110" s="5"/>
     </row>
@@ -3403,11 +3403,11 @@
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F112" s="6"/>
       <c r="G112" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H112" s="6"/>
     </row>
@@ -3419,11 +3419,11 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F113" s="7"/>
       <c r="G113" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H113" s="7"/>
     </row>
@@ -3435,11 +3435,11 @@
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
       <c r="E114" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F114" s="5"/>
       <c r="G114" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H114" s="5"/>
     </row>
@@ -3467,11 +3467,11 @@
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
       <c r="E116" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H116" s="6"/>
     </row>
@@ -3483,11 +3483,11 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F117" s="7"/>
       <c r="G117" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H117" s="7"/>
     </row>
@@ -3499,7 +3499,7 @@
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
@@ -3527,7 +3527,7 @@
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
@@ -3541,7 +3541,7 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>

</xml_diff>

<commit_message>
modified:   Input/Exam Timetable.xlsx 	modified:   __pycache__/class_set.cpython-311.pyc 	modified:   __pycache__/function_set.cpython-311.pyc 	modified:   main.ipynb 	modified:   try.ipynb 	modified:   "\347\233\243\350\200\203\346\231\202\351\226\223\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/Input/Exam Timetable.xlsx
+++ b/Input/Exam Timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784116AA-FA40-4B87-A0F2-F30B7D0E36C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EC6EC9-2DAB-441E-9120-1EDBAD6CAC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4131" yWindow="9154" windowWidth="24891" windowHeight="15035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -168,6 +168,9 @@
     </r>
   </si>
   <si>
+    <t>04/11/2021 (四)</t>
+  </si>
+  <si>
     <t>09/11/2021 (二)</t>
   </si>
   <si>
@@ -688,9 +691,6 @@
   </si>
   <si>
     <t>10:30am – 11:25am</t>
-  </si>
-  <si>
-    <t>04/11/2021 (四)</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1241,25 +1241,25 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>178</v>
+        <v>14</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -1267,25 +1267,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1316,16 +1316,16 @@
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1336,16 +1336,16 @@
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -1353,25 +1353,25 @@
         <v>0</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1402,19 +1402,19 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1422,16 +1422,16 @@
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1439,16 +1439,16 @@
         <v>0</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
@@ -1476,7 +1476,7 @@
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -1490,7 +1490,7 @@
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -1554,25 +1554,25 @@
         <v>10</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1603,16 +1603,16 @@
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1623,16 +1623,16 @@
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -1640,25 +1640,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1689,16 +1689,16 @@
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -1709,16 +1709,16 @@
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1726,16 +1726,16 @@
         <v>10</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -1763,7 +1763,7 @@
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -1777,7 +1777,7 @@
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
       <c r="E29" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -1841,23 +1841,23 @@
         <v>10</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G33" s="19"/>
       <c r="H33" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1889,23 +1889,23 @@
         <v>12</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1913,23 +1913,23 @@
         <v>9</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G36" s="21"/>
       <c r="H36" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1937,23 +1937,23 @@
         <v>10</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G37" s="19"/>
       <c r="H37" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -1985,23 +1985,23 @@
         <v>12</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2009,23 +2009,23 @@
         <v>9</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="F40" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G40" s="21"/>
       <c r="H40" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2039,7 +2039,7 @@
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
       <c r="H41" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2067,7 +2067,7 @@
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
       <c r="H43" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2081,7 +2081,7 @@
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
       <c r="H44" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2106,7 +2106,7 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="11" t="str">
         <f t="shared" ref="B47:H47" si="2">B2</f>
@@ -2142,25 +2142,25 @@
         <v>13</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2194,25 +2194,25 @@
         <v>12</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F50" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H50" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2220,25 +2220,25 @@
         <v>9</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2246,25 +2246,25 @@
         <v>13</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2298,25 +2298,25 @@
         <v>12</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2324,25 +2324,25 @@
         <v>9</v>
       </c>
       <c r="B55" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="D55" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2353,13 +2353,13 @@
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H56" s="19"/>
     </row>
@@ -2389,13 +2389,13 @@
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
       <c r="E58" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H58" s="20"/>
     </row>
@@ -2407,13 +2407,13 @@
       <c r="C59" s="21"/>
       <c r="D59" s="21"/>
       <c r="E59" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H59" s="21"/>
     </row>
@@ -2426,7 +2426,7 @@
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
       <c r="F60" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="19"/>
@@ -2454,7 +2454,7 @@
       <c r="D62" s="20"/>
       <c r="E62" s="20"/>
       <c r="F62" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
@@ -2468,7 +2468,7 @@
       <c r="D63" s="21"/>
       <c r="E63" s="21"/>
       <c r="F63" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G63" s="21"/>
       <c r="H63" s="21"/>
@@ -2495,7 +2495,7 @@
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
     </row>
-    <row r="66" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="11" t="str">
         <f t="shared" ref="B66:H66" si="3">B2</f>
@@ -2531,25 +2531,25 @@
         <v>13</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2583,25 +2583,25 @@
         <v>12</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D69" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F69" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>113</v>
-      </c>
       <c r="G69" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2609,25 +2609,25 @@
         <v>9</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2635,23 +2635,23 @@
         <v>13</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C71" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E71" s="5" t="s">
+      <c r="F71" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2683,23 +2683,23 @@
         <v>12</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G73" s="18"/>
       <c r="H73" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2707,23 +2707,23 @@
         <v>9</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2733,13 +2733,13 @@
       <c r="B75" s="18"/>
       <c r="C75" s="18"/>
       <c r="D75" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E75" s="18"/>
       <c r="F75" s="18"/>
       <c r="G75" s="18"/>
       <c r="H75" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2765,13 +2765,13 @@
       <c r="B77" s="18"/>
       <c r="C77" s="18"/>
       <c r="D77" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E77" s="18"/>
       <c r="F77" s="18"/>
       <c r="G77" s="18"/>
       <c r="H77" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2781,13 +2781,13 @@
       <c r="B78" s="18"/>
       <c r="C78" s="18"/>
       <c r="D78" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E78" s="18"/>
       <c r="F78" s="18"/>
       <c r="G78" s="18"/>
       <c r="H78" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2797,13 +2797,13 @@
       <c r="B79" s="18"/>
       <c r="C79" s="18"/>
       <c r="D79" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E79" s="18"/>
       <c r="F79" s="18"/>
       <c r="G79" s="18"/>
       <c r="H79" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2829,13 +2829,13 @@
       <c r="B81" s="18"/>
       <c r="C81" s="18"/>
       <c r="D81" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E81" s="18"/>
       <c r="F81" s="18"/>
       <c r="G81" s="18"/>
       <c r="H81" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2845,13 +2845,13 @@
       <c r="B82" s="18"/>
       <c r="C82" s="18"/>
       <c r="D82" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E82" s="18"/>
       <c r="F82" s="18"/>
       <c r="G82" s="18"/>
       <c r="H82" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2861,13 +2861,13 @@
       <c r="B83" s="18"/>
       <c r="C83" s="18"/>
       <c r="D83" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E83" s="18"/>
       <c r="F83" s="18"/>
       <c r="G83" s="18"/>
       <c r="H83" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2893,13 +2893,13 @@
       <c r="B85" s="18"/>
       <c r="C85" s="18"/>
       <c r="D85" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E85" s="18"/>
       <c r="F85" s="18"/>
       <c r="G85" s="18"/>
       <c r="H85" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2909,13 +2909,13 @@
       <c r="B86" s="18"/>
       <c r="C86" s="18"/>
       <c r="D86" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E86" s="18"/>
       <c r="F86" s="18"/>
       <c r="G86" s="18"/>
       <c r="H86" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -2925,7 +2925,7 @@
       <c r="B87" s="18"/>
       <c r="C87" s="18"/>
       <c r="D87" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E87" s="18"/>
       <c r="F87" s="18"/>
@@ -2953,7 +2953,7 @@
       <c r="B89" s="18"/>
       <c r="C89" s="18"/>
       <c r="D89" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E89" s="18"/>
       <c r="F89" s="18"/>
@@ -2967,7 +2967,7 @@
       <c r="B90" s="18"/>
       <c r="C90" s="18"/>
       <c r="D90" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
@@ -2996,7 +2996,7 @@
       <c r="G92" s="15"/>
       <c r="H92" s="15"/>
     </row>
-    <row r="93" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="11" t="str">
         <f t="shared" ref="B93:H93" si="4">B2</f>
@@ -3032,25 +3032,25 @@
         <v>13</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -3084,25 +3084,25 @@
         <v>12</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -3110,25 +3110,25 @@
         <v>9</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -3136,25 +3136,25 @@
         <v>13</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -3188,25 +3188,25 @@
         <v>12</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -3214,25 +3214,25 @@
         <v>9</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
@@ -3243,11 +3243,11 @@
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F102" s="5"/>
       <c r="G102" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H102" s="5"/>
     </row>
@@ -3275,11 +3275,11 @@
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H104" s="6"/>
     </row>
@@ -3291,11 +3291,11 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H105" s="7"/>
     </row>
@@ -3307,11 +3307,11 @@
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
       <c r="E106" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F106" s="5"/>
       <c r="G106" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H106" s="5"/>
     </row>
@@ -3339,11 +3339,11 @@
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H108" s="6"/>
     </row>
@@ -3355,11 +3355,11 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H109" s="7"/>
     </row>
@@ -3371,11 +3371,11 @@
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F110" s="5"/>
       <c r="G110" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H110" s="5"/>
     </row>
@@ -3403,11 +3403,11 @@
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F112" s="6"/>
       <c r="G112" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H112" s="6"/>
     </row>
@@ -3419,11 +3419,11 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F113" s="7"/>
       <c r="G113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H113" s="7"/>
     </row>
@@ -3435,11 +3435,11 @@
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
       <c r="E114" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F114" s="5"/>
       <c r="G114" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H114" s="5"/>
     </row>
@@ -3467,11 +3467,11 @@
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
       <c r="E116" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H116" s="6"/>
     </row>
@@ -3483,11 +3483,11 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F117" s="7"/>
       <c r="G117" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H117" s="7"/>
     </row>
@@ -3499,7 +3499,7 @@
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
@@ -3527,7 +3527,7 @@
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
@@ -3541,7 +3541,7 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>

</xml_diff>